<commit_message>
Updated Gantt chart with progress
</commit_message>
<xml_diff>
--- a/documentation/Interim Report/Gantt Chart.xlsx
+++ b/documentation/Interim Report/Gantt Chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23426"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domin\Documents\University\CO3201\documentation\Interim Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06AFD537-FA10-4A90-AE35-6A1BAB865961}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{027A9818-6620-4C2F-8363-94FD00BBB029}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25490" yWindow="-4470" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -798,6 +798,99 @@
     <xf numFmtId="9" fontId="5" fillId="20" borderId="0" xfId="6" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="13" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="13" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="13" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="14" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="14" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="15" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="15" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="16" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="17" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="17" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="16" fontId="9" fillId="19" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -813,9 +906,6 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -834,101 +924,11 @@
     <xf numFmtId="16" fontId="13" fillId="19" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="9" fillId="17" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="16" fontId="9" fillId="18" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="16" fontId="9" fillId="18" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="16" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="17" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="15" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="15" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="14" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="14" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="13" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="13" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="13" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1341,8 +1341,8 @@
   </sheetPr>
   <dimension ref="B1:BP39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="AQ15" sqref="AQ15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1368,62 +1368,62 @@
       <c r="H1" s="8"/>
     </row>
     <row r="2" spans="2:68" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="34" t="s">
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="35"/>
+      <c r="H2" s="66"/>
       <c r="I2" s="25">
         <v>57</v>
       </c>
       <c r="K2" s="9"/>
-      <c r="L2" s="67" t="s">
+      <c r="L2" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="68"/>
-      <c r="N2" s="68"/>
-      <c r="O2" s="68"/>
-      <c r="P2" s="69"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="35"/>
       <c r="Q2" s="10"/>
-      <c r="R2" s="67" t="s">
+      <c r="R2" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="70"/>
-      <c r="T2" s="70"/>
-      <c r="U2" s="69"/>
+      <c r="S2" s="36"/>
+      <c r="T2" s="36"/>
+      <c r="U2" s="35"/>
       <c r="V2" s="11"/>
-      <c r="W2" s="65" t="s">
+      <c r="W2" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="X2" s="66"/>
-      <c r="Y2" s="66"/>
-      <c r="Z2" s="71"/>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="32"/>
+      <c r="Z2" s="37"/>
       <c r="AA2" s="12"/>
-      <c r="AB2" s="72" t="s">
+      <c r="AB2" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="AC2" s="73"/>
-      <c r="AD2" s="73"/>
-      <c r="AE2" s="73"/>
-      <c r="AF2" s="73"/>
-      <c r="AG2" s="73"/>
-      <c r="AH2" s="74"/>
+      <c r="AC2" s="39"/>
+      <c r="AD2" s="39"/>
+      <c r="AE2" s="39"/>
+      <c r="AF2" s="39"/>
+      <c r="AG2" s="39"/>
+      <c r="AH2" s="40"/>
       <c r="AI2" s="13"/>
-      <c r="AJ2" s="65" t="s">
+      <c r="AJ2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="AK2" s="66"/>
-      <c r="AL2" s="66"/>
-      <c r="AM2" s="66"/>
-      <c r="AN2" s="66"/>
-      <c r="AO2" s="66"/>
-      <c r="AP2" s="66"/>
-      <c r="AQ2" s="66"/>
+      <c r="AK2" s="32"/>
+      <c r="AL2" s="32"/>
+      <c r="AM2" s="32"/>
+      <c r="AN2" s="32"/>
+      <c r="AO2" s="32"/>
+      <c r="AP2" s="32"/>
+      <c r="AQ2" s="32"/>
     </row>
     <row r="3" spans="2:68" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C3"/>
@@ -1454,23 +1454,23 @@
       <c r="AB3"/>
     </row>
     <row r="4" spans="2:68" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="62" t="s">
+      <c r="B4" s="67" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="67"/>
+      <c r="D4" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="62" t="s">
+      <c r="E4" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="62" t="s">
+      <c r="F4" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="62" t="s">
+      <c r="G4" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="64" t="s">
+      <c r="H4" s="50" t="s">
         <v>10</v>
       </c>
       <c r="I4" s="15" t="s">
@@ -1486,140 +1486,140 @@
       <c r="O4" s="14"/>
     </row>
     <row r="5" spans="2:68" s="7" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="64"/>
-      <c r="I5" s="58">
+      <c r="B5" s="67"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="42">
         <v>44120</v>
       </c>
-      <c r="J5" s="59"/>
-      <c r="K5" s="59">
+      <c r="J5" s="43"/>
+      <c r="K5" s="43">
         <v>44127</v>
       </c>
-      <c r="L5" s="60"/>
-      <c r="M5" s="54">
+      <c r="L5" s="44"/>
+      <c r="M5" s="45">
         <v>44134</v>
       </c>
-      <c r="N5" s="54"/>
-      <c r="O5" s="54">
+      <c r="N5" s="45"/>
+      <c r="O5" s="45">
         <v>44141</v>
       </c>
-      <c r="P5" s="54"/>
-      <c r="Q5" s="54">
+      <c r="P5" s="45"/>
+      <c r="Q5" s="45">
         <v>44148</v>
       </c>
-      <c r="R5" s="54"/>
-      <c r="S5" s="55">
+      <c r="R5" s="45"/>
+      <c r="S5" s="51">
         <v>44155</v>
       </c>
-      <c r="T5" s="55"/>
-      <c r="U5" s="54">
+      <c r="T5" s="51"/>
+      <c r="U5" s="45">
         <v>44162</v>
       </c>
-      <c r="V5" s="56"/>
-      <c r="W5" s="51">
+      <c r="V5" s="52"/>
+      <c r="W5" s="53">
         <v>44169</v>
       </c>
-      <c r="X5" s="51"/>
-      <c r="Y5" s="50">
+      <c r="X5" s="53"/>
+      <c r="Y5" s="54">
         <v>44176</v>
       </c>
-      <c r="Z5" s="50"/>
-      <c r="AA5" s="51">
+      <c r="Z5" s="54"/>
+      <c r="AA5" s="53">
         <v>44183</v>
       </c>
-      <c r="AB5" s="51"/>
-      <c r="AC5" s="50">
+      <c r="AB5" s="53"/>
+      <c r="AC5" s="54">
         <v>44190</v>
       </c>
-      <c r="AD5" s="52"/>
-      <c r="AE5" s="53">
+      <c r="AD5" s="55"/>
+      <c r="AE5" s="56">
         <v>44197</v>
       </c>
-      <c r="AF5" s="47"/>
-      <c r="AG5" s="48">
+      <c r="AF5" s="57"/>
+      <c r="AG5" s="58">
         <v>44204</v>
       </c>
-      <c r="AH5" s="48"/>
-      <c r="AI5" s="47">
+      <c r="AH5" s="58"/>
+      <c r="AI5" s="57">
         <v>44211</v>
       </c>
-      <c r="AJ5" s="47"/>
-      <c r="AK5" s="48">
+      <c r="AJ5" s="57"/>
+      <c r="AK5" s="58">
         <v>44218</v>
       </c>
-      <c r="AL5" s="48"/>
-      <c r="AM5" s="47">
+      <c r="AL5" s="58"/>
+      <c r="AM5" s="57">
         <v>44225</v>
       </c>
-      <c r="AN5" s="47"/>
-      <c r="AO5" s="49">
+      <c r="AN5" s="57"/>
+      <c r="AO5" s="59">
         <v>44232</v>
       </c>
-      <c r="AP5" s="43"/>
-      <c r="AQ5" s="44">
+      <c r="AP5" s="60"/>
+      <c r="AQ5" s="61">
         <v>44239</v>
       </c>
-      <c r="AR5" s="44"/>
-      <c r="AS5" s="43">
+      <c r="AR5" s="61"/>
+      <c r="AS5" s="60">
         <v>44246</v>
       </c>
-      <c r="AT5" s="43"/>
-      <c r="AU5" s="44">
+      <c r="AT5" s="60"/>
+      <c r="AU5" s="61">
         <v>44253</v>
       </c>
-      <c r="AV5" s="44"/>
-      <c r="AW5" s="45">
+      <c r="AV5" s="61"/>
+      <c r="AW5" s="73">
         <v>44260</v>
       </c>
-      <c r="AX5" s="46"/>
-      <c r="AY5" s="39">
+      <c r="AX5" s="74"/>
+      <c r="AY5" s="69">
         <v>44267</v>
       </c>
-      <c r="AZ5" s="39"/>
-      <c r="BA5" s="46">
+      <c r="AZ5" s="69"/>
+      <c r="BA5" s="74">
         <v>44274</v>
       </c>
-      <c r="BB5" s="46"/>
-      <c r="BC5" s="39">
+      <c r="BB5" s="74"/>
+      <c r="BC5" s="69">
         <v>44281</v>
       </c>
-      <c r="BD5" s="40"/>
-      <c r="BE5" s="41">
+      <c r="BD5" s="70"/>
+      <c r="BE5" s="71">
         <v>44288</v>
       </c>
-      <c r="BF5" s="31"/>
-      <c r="BG5" s="42">
+      <c r="BF5" s="62"/>
+      <c r="BG5" s="72">
         <v>44295</v>
       </c>
-      <c r="BH5" s="42"/>
-      <c r="BI5" s="31">
+      <c r="BH5" s="72"/>
+      <c r="BI5" s="62">
         <v>44302</v>
       </c>
-      <c r="BJ5" s="31"/>
-      <c r="BK5" s="42">
+      <c r="BJ5" s="62"/>
+      <c r="BK5" s="72">
         <v>44309</v>
       </c>
-      <c r="BL5" s="42"/>
-      <c r="BM5" s="31">
+      <c r="BL5" s="72"/>
+      <c r="BM5" s="62">
         <v>44316</v>
       </c>
-      <c r="BN5" s="32"/>
+      <c r="BN5" s="63"/>
       <c r="BO5" s="16"/>
       <c r="BP5" s="6"/>
     </row>
     <row r="6" spans="2:68" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="63"/>
-      <c r="H6" s="63"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
       <c r="I6" s="21">
         <v>1</v>
       </c>
@@ -1802,10 +1802,10 @@
       </c>
     </row>
     <row r="7" spans="2:68" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="36"/>
+      <c r="C7" s="46"/>
       <c r="D7" s="4">
         <v>8</v>
       </c>
@@ -1825,10 +1825,10 @@
       <c r="J7" s="24"/>
     </row>
     <row r="8" spans="2:68" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="36"/>
+      <c r="C8" s="46"/>
       <c r="D8" s="4">
         <v>41</v>
       </c>
@@ -1844,10 +1844,10 @@
       <c r="J8" s="23"/>
     </row>
     <row r="9" spans="2:68" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="36"/>
+      <c r="C9" s="46"/>
       <c r="D9" s="4">
         <v>1</v>
       </c>
@@ -1863,10 +1863,10 @@
       <c r="J9" s="23"/>
     </row>
     <row r="10" spans="2:68" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="61" t="s">
+      <c r="B10" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="61"/>
+      <c r="C10" s="47"/>
       <c r="D10" s="29">
         <v>1</v>
       </c>
@@ -1978,10 +1978,10 @@
       <c r="J14" s="23"/>
     </row>
     <row r="15" spans="2:68" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="61" t="s">
+      <c r="B15" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="61"/>
+      <c r="C15" s="47"/>
       <c r="D15" s="29">
         <v>5</v>
       </c>
@@ -2133,7 +2133,7 @@
         <v>2</v>
       </c>
       <c r="H21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21" s="23"/>
       <c r="J21" s="23"/>
@@ -2147,7 +2147,7 @@
         <v>17</v>
       </c>
       <c r="E22" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F22" s="4">
         <v>17</v>
@@ -2162,10 +2162,10 @@
       <c r="J22" s="23"/>
     </row>
     <row r="23" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="61" t="s">
+      <c r="B23" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="61"/>
+      <c r="C23" s="47"/>
       <c r="D23" s="29">
         <v>19</v>
       </c>
@@ -2333,10 +2333,10 @@
       <c r="J31" s="23"/>
     </row>
     <row r="32" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="61" t="s">
+      <c r="B32" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C32" s="61"/>
+      <c r="C32" s="47"/>
       <c r="D32" s="29">
         <v>33</v>
       </c>
@@ -2409,10 +2409,10 @@
       <c r="J35" s="23"/>
     </row>
     <row r="36" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="57" t="s">
+      <c r="B36" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="57"/>
+      <c r="C36" s="41"/>
       <c r="D36" s="29">
         <v>41</v>
       </c>
@@ -2486,40 +2486,6 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="AJ2:AQ2"/>
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="AB2:AH2"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="H4:H6"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="AK5:AL5"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="AO5:AP5"/>
-    <mergeCell ref="AQ5:AR5"/>
     <mergeCell ref="BM5:BN5"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="G2:H2"/>
@@ -2536,6 +2502,40 @@
     <mergeCell ref="AW5:AX5"/>
     <mergeCell ref="AY5:AZ5"/>
     <mergeCell ref="BA5:BB5"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="AK5:AL5"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="AO5:AP5"/>
+    <mergeCell ref="AQ5:AR5"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="AJ2:AQ2"/>
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="AB2:AH2"/>
   </mergeCells>
   <conditionalFormatting sqref="I7:BP39">
     <cfRule type="expression" dxfId="9" priority="1">

</xml_diff>

<commit_message>
Finished equipment package panel UI
</commit_message>
<xml_diff>
--- a/documentation/Interim Report/Gantt Chart.xlsx
+++ b/documentation/Interim Report/Gantt Chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domin\Documents\University\CO3201\documentation\Interim Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B75605-1F76-4631-A439-C6FA336B0122}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE6D8D3-82BC-4C65-AB7C-7661718176F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25490" yWindow="-4470" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -798,6 +798,99 @@
     <xf numFmtId="9" fontId="5" fillId="20" borderId="0" xfId="6" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="13" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="13" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="13" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="14" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="14" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="15" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="15" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="16" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="17" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="17" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="16" fontId="9" fillId="19" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -813,9 +906,6 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -834,101 +924,11 @@
     <xf numFmtId="16" fontId="13" fillId="19" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="9" fillId="17" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="16" fontId="9" fillId="18" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="16" fontId="9" fillId="18" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="16" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="17" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="15" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="15" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="14" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="14" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="13" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="13" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="13" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1342,7 +1342,7 @@
   <dimension ref="B1:BP39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+      <selection activeCell="AR17" sqref="AR17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1368,62 +1368,62 @@
       <c r="H1" s="8"/>
     </row>
     <row r="2" spans="2:68" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="34" t="s">
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="35"/>
+      <c r="H2" s="66"/>
       <c r="I2" s="25">
         <v>57</v>
       </c>
       <c r="K2" s="9"/>
-      <c r="L2" s="67" t="s">
+      <c r="L2" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="68"/>
-      <c r="N2" s="68"/>
-      <c r="O2" s="68"/>
-      <c r="P2" s="69"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="35"/>
       <c r="Q2" s="10"/>
-      <c r="R2" s="67" t="s">
+      <c r="R2" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="70"/>
-      <c r="T2" s="70"/>
-      <c r="U2" s="69"/>
+      <c r="S2" s="36"/>
+      <c r="T2" s="36"/>
+      <c r="U2" s="35"/>
       <c r="V2" s="11"/>
-      <c r="W2" s="65" t="s">
+      <c r="W2" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="X2" s="66"/>
-      <c r="Y2" s="66"/>
-      <c r="Z2" s="71"/>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="32"/>
+      <c r="Z2" s="37"/>
       <c r="AA2" s="12"/>
-      <c r="AB2" s="72" t="s">
+      <c r="AB2" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="AC2" s="73"/>
-      <c r="AD2" s="73"/>
-      <c r="AE2" s="73"/>
-      <c r="AF2" s="73"/>
-      <c r="AG2" s="73"/>
-      <c r="AH2" s="74"/>
+      <c r="AC2" s="39"/>
+      <c r="AD2" s="39"/>
+      <c r="AE2" s="39"/>
+      <c r="AF2" s="39"/>
+      <c r="AG2" s="39"/>
+      <c r="AH2" s="40"/>
       <c r="AI2" s="13"/>
-      <c r="AJ2" s="65" t="s">
+      <c r="AJ2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="AK2" s="66"/>
-      <c r="AL2" s="66"/>
-      <c r="AM2" s="66"/>
-      <c r="AN2" s="66"/>
-      <c r="AO2" s="66"/>
-      <c r="AP2" s="66"/>
-      <c r="AQ2" s="66"/>
+      <c r="AK2" s="32"/>
+      <c r="AL2" s="32"/>
+      <c r="AM2" s="32"/>
+      <c r="AN2" s="32"/>
+      <c r="AO2" s="32"/>
+      <c r="AP2" s="32"/>
+      <c r="AQ2" s="32"/>
     </row>
     <row r="3" spans="2:68" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C3"/>
@@ -1454,23 +1454,23 @@
       <c r="AB3"/>
     </row>
     <row r="4" spans="2:68" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="62" t="s">
+      <c r="B4" s="67" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="67"/>
+      <c r="D4" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="62" t="s">
+      <c r="E4" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="62" t="s">
+      <c r="F4" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="62" t="s">
+      <c r="G4" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="64" t="s">
+      <c r="H4" s="50" t="s">
         <v>10</v>
       </c>
       <c r="I4" s="15" t="s">
@@ -1486,140 +1486,140 @@
       <c r="O4" s="14"/>
     </row>
     <row r="5" spans="2:68" s="7" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="64"/>
-      <c r="I5" s="58">
+      <c r="B5" s="67"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="42">
         <v>44120</v>
       </c>
-      <c r="J5" s="59"/>
-      <c r="K5" s="59">
+      <c r="J5" s="43"/>
+      <c r="K5" s="43">
         <v>44127</v>
       </c>
-      <c r="L5" s="60"/>
-      <c r="M5" s="54">
+      <c r="L5" s="44"/>
+      <c r="M5" s="45">
         <v>44134</v>
       </c>
-      <c r="N5" s="54"/>
-      <c r="O5" s="54">
+      <c r="N5" s="45"/>
+      <c r="O5" s="45">
         <v>44141</v>
       </c>
-      <c r="P5" s="54"/>
-      <c r="Q5" s="54">
+      <c r="P5" s="45"/>
+      <c r="Q5" s="45">
         <v>44148</v>
       </c>
-      <c r="R5" s="54"/>
-      <c r="S5" s="55">
+      <c r="R5" s="45"/>
+      <c r="S5" s="51">
         <v>44155</v>
       </c>
-      <c r="T5" s="55"/>
-      <c r="U5" s="54">
+      <c r="T5" s="51"/>
+      <c r="U5" s="45">
         <v>44162</v>
       </c>
-      <c r="V5" s="56"/>
-      <c r="W5" s="51">
+      <c r="V5" s="52"/>
+      <c r="W5" s="53">
         <v>44169</v>
       </c>
-      <c r="X5" s="51"/>
-      <c r="Y5" s="50">
+      <c r="X5" s="53"/>
+      <c r="Y5" s="54">
         <v>44176</v>
       </c>
-      <c r="Z5" s="50"/>
-      <c r="AA5" s="51">
+      <c r="Z5" s="54"/>
+      <c r="AA5" s="53">
         <v>44183</v>
       </c>
-      <c r="AB5" s="51"/>
-      <c r="AC5" s="50">
+      <c r="AB5" s="53"/>
+      <c r="AC5" s="54">
         <v>44190</v>
       </c>
-      <c r="AD5" s="52"/>
-      <c r="AE5" s="53">
+      <c r="AD5" s="55"/>
+      <c r="AE5" s="56">
         <v>44197</v>
       </c>
-      <c r="AF5" s="47"/>
-      <c r="AG5" s="48">
+      <c r="AF5" s="57"/>
+      <c r="AG5" s="58">
         <v>44204</v>
       </c>
-      <c r="AH5" s="48"/>
-      <c r="AI5" s="47">
+      <c r="AH5" s="58"/>
+      <c r="AI5" s="57">
         <v>44211</v>
       </c>
-      <c r="AJ5" s="47"/>
-      <c r="AK5" s="48">
+      <c r="AJ5" s="57"/>
+      <c r="AK5" s="58">
         <v>44218</v>
       </c>
-      <c r="AL5" s="48"/>
-      <c r="AM5" s="47">
+      <c r="AL5" s="58"/>
+      <c r="AM5" s="57">
         <v>44225</v>
       </c>
-      <c r="AN5" s="47"/>
-      <c r="AO5" s="49">
+      <c r="AN5" s="57"/>
+      <c r="AO5" s="59">
         <v>44232</v>
       </c>
-      <c r="AP5" s="43"/>
-      <c r="AQ5" s="44">
+      <c r="AP5" s="60"/>
+      <c r="AQ5" s="61">
         <v>44239</v>
       </c>
-      <c r="AR5" s="44"/>
-      <c r="AS5" s="43">
+      <c r="AR5" s="61"/>
+      <c r="AS5" s="60">
         <v>44246</v>
       </c>
-      <c r="AT5" s="43"/>
-      <c r="AU5" s="44">
+      <c r="AT5" s="60"/>
+      <c r="AU5" s="61">
         <v>44253</v>
       </c>
-      <c r="AV5" s="44"/>
-      <c r="AW5" s="45">
+      <c r="AV5" s="61"/>
+      <c r="AW5" s="73">
         <v>44260</v>
       </c>
-      <c r="AX5" s="46"/>
-      <c r="AY5" s="39">
+      <c r="AX5" s="74"/>
+      <c r="AY5" s="69">
         <v>44267</v>
       </c>
-      <c r="AZ5" s="39"/>
-      <c r="BA5" s="46">
+      <c r="AZ5" s="69"/>
+      <c r="BA5" s="74">
         <v>44274</v>
       </c>
-      <c r="BB5" s="46"/>
-      <c r="BC5" s="39">
+      <c r="BB5" s="74"/>
+      <c r="BC5" s="69">
         <v>44281</v>
       </c>
-      <c r="BD5" s="40"/>
-      <c r="BE5" s="41">
+      <c r="BD5" s="70"/>
+      <c r="BE5" s="71">
         <v>44288</v>
       </c>
-      <c r="BF5" s="31"/>
-      <c r="BG5" s="42">
+      <c r="BF5" s="62"/>
+      <c r="BG5" s="72">
         <v>44295</v>
       </c>
-      <c r="BH5" s="42"/>
-      <c r="BI5" s="31">
+      <c r="BH5" s="72"/>
+      <c r="BI5" s="62">
         <v>44302</v>
       </c>
-      <c r="BJ5" s="31"/>
-      <c r="BK5" s="42">
+      <c r="BJ5" s="62"/>
+      <c r="BK5" s="72">
         <v>44309</v>
       </c>
-      <c r="BL5" s="42"/>
-      <c r="BM5" s="31">
+      <c r="BL5" s="72"/>
+      <c r="BM5" s="62">
         <v>44316</v>
       </c>
-      <c r="BN5" s="32"/>
+      <c r="BN5" s="63"/>
       <c r="BO5" s="16"/>
       <c r="BP5" s="6"/>
     </row>
     <row r="6" spans="2:68" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="63"/>
-      <c r="H6" s="63"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
       <c r="I6" s="21">
         <v>1</v>
       </c>
@@ -1802,10 +1802,10 @@
       </c>
     </row>
     <row r="7" spans="2:68" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="36"/>
+      <c r="C7" s="46"/>
       <c r="D7" s="4">
         <v>8</v>
       </c>
@@ -1825,10 +1825,10 @@
       <c r="J7" s="24"/>
     </row>
     <row r="8" spans="2:68" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="36"/>
+      <c r="C8" s="46"/>
       <c r="D8" s="4">
         <v>41</v>
       </c>
@@ -1844,10 +1844,10 @@
       <c r="J8" s="23"/>
     </row>
     <row r="9" spans="2:68" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="36"/>
+      <c r="C9" s="46"/>
       <c r="D9" s="4">
         <v>1</v>
       </c>
@@ -1863,10 +1863,10 @@
       <c r="J9" s="23"/>
     </row>
     <row r="10" spans="2:68" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="61" t="s">
+      <c r="B10" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="61"/>
+      <c r="C10" s="47"/>
       <c r="D10" s="29">
         <v>1</v>
       </c>
@@ -1978,10 +1978,10 @@
       <c r="J14" s="23"/>
     </row>
     <row r="15" spans="2:68" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="61" t="s">
+      <c r="B15" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="61"/>
+      <c r="C15" s="47"/>
       <c r="D15" s="29">
         <v>5</v>
       </c>
@@ -1992,10 +1992,10 @@
         <v>5</v>
       </c>
       <c r="G15" s="29">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H15" s="30">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="I15" s="23"/>
       <c r="J15" s="23"/>
@@ -2150,30 +2150,34 @@
         <v>2</v>
       </c>
       <c r="F22" s="4">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="G22" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" s="23"/>
       <c r="J22" s="23"/>
     </row>
     <row r="23" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="61" t="s">
+      <c r="B23" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="61"/>
+      <c r="C23" s="47"/>
       <c r="D23" s="29">
         <v>19</v>
       </c>
       <c r="E23" s="29">
         <v>14</v>
       </c>
-      <c r="F23" s="29"/>
-      <c r="G23" s="29"/>
+      <c r="F23" s="29">
+        <v>27</v>
+      </c>
+      <c r="G23" s="29">
+        <v>6</v>
+      </c>
       <c r="H23" s="30">
         <v>0</v>
       </c>
@@ -2191,8 +2195,12 @@
       <c r="E24" s="4">
         <v>1</v>
       </c>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
+      <c r="F24" s="4">
+        <v>27</v>
+      </c>
+      <c r="G24" s="4">
+        <v>1</v>
+      </c>
       <c r="H24" s="5">
         <v>0</v>
       </c>
@@ -2333,10 +2341,10 @@
       <c r="J31" s="23"/>
     </row>
     <row r="32" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="61" t="s">
+      <c r="B32" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="61"/>
+      <c r="C32" s="47"/>
       <c r="D32" s="29">
         <v>33</v>
       </c>
@@ -2409,10 +2417,10 @@
       <c r="J35" s="23"/>
     </row>
     <row r="36" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="57" t="s">
+      <c r="B36" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="C36" s="57"/>
+      <c r="C36" s="41"/>
       <c r="D36" s="29">
         <v>41</v>
       </c>
@@ -2486,40 +2494,6 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="AJ2:AQ2"/>
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="AB2:AH2"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="H4:H6"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="AK5:AL5"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="AO5:AP5"/>
-    <mergeCell ref="AQ5:AR5"/>
     <mergeCell ref="BM5:BN5"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="G2:H2"/>
@@ -2536,6 +2510,40 @@
     <mergeCell ref="AW5:AX5"/>
     <mergeCell ref="AY5:AZ5"/>
     <mergeCell ref="BA5:BB5"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="AK5:AL5"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="AO5:AP5"/>
+    <mergeCell ref="AQ5:AR5"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="AJ2:AQ2"/>
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="AB2:AH2"/>
   </mergeCells>
   <conditionalFormatting sqref="I7:BP39">
     <cfRule type="expression" dxfId="9" priority="1">

</xml_diff>

<commit_message>
Hid background description. Moved to tabs for selecting background skills. Moved ref for large avatar size
</commit_message>
<xml_diff>
--- a/documentation/Interim Report/Gantt Chart.xlsx
+++ b/documentation/Interim Report/Gantt Chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domin\Documents\University\CO3201\documentation\Interim Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE6D8D3-82BC-4C65-AB7C-7661718176F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70031760-9210-4A73-ACEE-3FD388BBD830}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1342,7 +1342,7 @@
   <dimension ref="B1:BP39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="AR17" sqref="AR17"/>
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2199,10 +2199,10 @@
         <v>27</v>
       </c>
       <c r="G24" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H24" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24" s="23"/>
       <c r="J24" s="23"/>
@@ -2218,8 +2218,12 @@
       <c r="E25" s="4">
         <v>2</v>
       </c>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
+      <c r="F25" s="4">
+        <v>32</v>
+      </c>
+      <c r="G25" s="4">
+        <v>3</v>
+      </c>
       <c r="H25" s="5">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Background functionality complete except attribute bonuses and system skill acquisition which will be added after skill functionality
</commit_message>
<xml_diff>
--- a/documentation/Interim Report/Gantt Chart.xlsx
+++ b/documentation/Interim Report/Gantt Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domin\Documents\University\CO3201\documentation\Interim Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70031760-9210-4A73-ACEE-3FD388BBD830}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65120388-E077-4EC6-A5D4-84283279516D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1342,7 +1342,7 @@
   <dimension ref="B1:BP39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+      <selection activeCell="S23" sqref="S23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1819,7 +1819,7 @@
         <v>5</v>
       </c>
       <c r="H7" s="5">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="I7" s="23"/>
       <c r="J7" s="24"/>
@@ -2176,7 +2176,7 @@
         <v>27</v>
       </c>
       <c r="G23" s="29">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="H23" s="30">
         <v>0</v>
@@ -2199,7 +2199,7 @@
         <v>27</v>
       </c>
       <c r="G24" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H24" s="5">
         <v>1</v>
@@ -2219,13 +2219,13 @@
         <v>2</v>
       </c>
       <c r="F25" s="4">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G25" s="4">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="H25" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25" s="23"/>
       <c r="J25" s="23"/>
@@ -2241,8 +2241,12 @@
       <c r="E26" s="4">
         <v>2</v>
       </c>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
+      <c r="F26" s="4">
+        <v>41</v>
+      </c>
+      <c r="G26" s="4">
+        <v>1</v>
+      </c>
       <c r="H26" s="5">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Fixed bug whereby UI showed that skills earnt from backgrounds could be unassigned
</commit_message>
<xml_diff>
--- a/documentation/Interim Report/Gantt Chart.xlsx
+++ b/documentation/Interim Report/Gantt Chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domin\Documents\University\CO3201\documentation\Interim Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65120388-E077-4EC6-A5D4-84283279516D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBFA8B8B-A920-4F0E-A999-B91AB9006664}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -798,6 +798,108 @@
     <xf numFmtId="9" fontId="5" fillId="20" borderId="0" xfId="6" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="9" fillId="19" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="19" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="12" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="19" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="19" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="17" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="18" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="18" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="16" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="17" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="15" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="15" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="14" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="14" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="13" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="13" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="13" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -827,108 +929,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="13" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="13" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="13" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="14" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="14" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="15" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="15" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="16" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="17" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="17" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="19" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="19" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="12" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="19" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="19" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="18" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="18" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1342,7 +1342,7 @@
   <dimension ref="B1:BP39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="S23" sqref="S23"/>
+      <selection activeCell="AW14" sqref="AW14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1368,62 +1368,62 @@
       <c r="H1" s="8"/>
     </row>
     <row r="2" spans="2:68" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="65" t="s">
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="66"/>
+      <c r="H2" s="35"/>
       <c r="I2" s="25">
         <v>57</v>
       </c>
       <c r="K2" s="9"/>
-      <c r="L2" s="33" t="s">
+      <c r="L2" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="35"/>
+      <c r="M2" s="68"/>
+      <c r="N2" s="68"/>
+      <c r="O2" s="68"/>
+      <c r="P2" s="69"/>
       <c r="Q2" s="10"/>
-      <c r="R2" s="33" t="s">
+      <c r="R2" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="36"/>
-      <c r="T2" s="36"/>
-      <c r="U2" s="35"/>
+      <c r="S2" s="70"/>
+      <c r="T2" s="70"/>
+      <c r="U2" s="69"/>
       <c r="V2" s="11"/>
-      <c r="W2" s="31" t="s">
+      <c r="W2" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="X2" s="32"/>
-      <c r="Y2" s="32"/>
-      <c r="Z2" s="37"/>
+      <c r="X2" s="66"/>
+      <c r="Y2" s="66"/>
+      <c r="Z2" s="71"/>
       <c r="AA2" s="12"/>
-      <c r="AB2" s="38" t="s">
+      <c r="AB2" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="AC2" s="39"/>
-      <c r="AD2" s="39"/>
-      <c r="AE2" s="39"/>
-      <c r="AF2" s="39"/>
-      <c r="AG2" s="39"/>
-      <c r="AH2" s="40"/>
+      <c r="AC2" s="73"/>
+      <c r="AD2" s="73"/>
+      <c r="AE2" s="73"/>
+      <c r="AF2" s="73"/>
+      <c r="AG2" s="73"/>
+      <c r="AH2" s="74"/>
       <c r="AI2" s="13"/>
-      <c r="AJ2" s="31" t="s">
+      <c r="AJ2" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="AK2" s="32"/>
-      <c r="AL2" s="32"/>
-      <c r="AM2" s="32"/>
-      <c r="AN2" s="32"/>
-      <c r="AO2" s="32"/>
-      <c r="AP2" s="32"/>
-      <c r="AQ2" s="32"/>
+      <c r="AK2" s="66"/>
+      <c r="AL2" s="66"/>
+      <c r="AM2" s="66"/>
+      <c r="AN2" s="66"/>
+      <c r="AO2" s="66"/>
+      <c r="AP2" s="66"/>
+      <c r="AQ2" s="66"/>
     </row>
     <row r="3" spans="2:68" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C3"/>
@@ -1454,23 +1454,23 @@
       <c r="AB3"/>
     </row>
     <row r="4" spans="2:68" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="67" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="67"/>
-      <c r="D4" s="48" t="s">
+      <c r="B4" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="37"/>
+      <c r="D4" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="48" t="s">
+      <c r="E4" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="48" t="s">
+      <c r="F4" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="48" t="s">
+      <c r="G4" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="50" t="s">
+      <c r="H4" s="64" t="s">
         <v>10</v>
       </c>
       <c r="I4" s="15" t="s">
@@ -1486,140 +1486,140 @@
       <c r="O4" s="14"/>
     </row>
     <row r="5" spans="2:68" s="7" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="67"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="42">
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="58">
         <v>44120</v>
       </c>
-      <c r="J5" s="43"/>
-      <c r="K5" s="43">
+      <c r="J5" s="59"/>
+      <c r="K5" s="59">
         <v>44127</v>
       </c>
-      <c r="L5" s="44"/>
-      <c r="M5" s="45">
+      <c r="L5" s="60"/>
+      <c r="M5" s="54">
         <v>44134</v>
       </c>
-      <c r="N5" s="45"/>
-      <c r="O5" s="45">
+      <c r="N5" s="54"/>
+      <c r="O5" s="54">
         <v>44141</v>
       </c>
-      <c r="P5" s="45"/>
-      <c r="Q5" s="45">
+      <c r="P5" s="54"/>
+      <c r="Q5" s="54">
         <v>44148</v>
       </c>
-      <c r="R5" s="45"/>
-      <c r="S5" s="51">
+      <c r="R5" s="54"/>
+      <c r="S5" s="55">
         <v>44155</v>
       </c>
-      <c r="T5" s="51"/>
-      <c r="U5" s="45">
+      <c r="T5" s="55"/>
+      <c r="U5" s="54">
         <v>44162</v>
       </c>
-      <c r="V5" s="52"/>
-      <c r="W5" s="53">
+      <c r="V5" s="56"/>
+      <c r="W5" s="51">
         <v>44169</v>
       </c>
-      <c r="X5" s="53"/>
-      <c r="Y5" s="54">
+      <c r="X5" s="51"/>
+      <c r="Y5" s="50">
         <v>44176</v>
       </c>
-      <c r="Z5" s="54"/>
-      <c r="AA5" s="53">
+      <c r="Z5" s="50"/>
+      <c r="AA5" s="51">
         <v>44183</v>
       </c>
-      <c r="AB5" s="53"/>
-      <c r="AC5" s="54">
+      <c r="AB5" s="51"/>
+      <c r="AC5" s="50">
         <v>44190</v>
       </c>
-      <c r="AD5" s="55"/>
-      <c r="AE5" s="56">
+      <c r="AD5" s="52"/>
+      <c r="AE5" s="53">
         <v>44197</v>
       </c>
-      <c r="AF5" s="57"/>
-      <c r="AG5" s="58">
+      <c r="AF5" s="47"/>
+      <c r="AG5" s="48">
         <v>44204</v>
       </c>
-      <c r="AH5" s="58"/>
-      <c r="AI5" s="57">
+      <c r="AH5" s="48"/>
+      <c r="AI5" s="47">
         <v>44211</v>
       </c>
-      <c r="AJ5" s="57"/>
-      <c r="AK5" s="58">
+      <c r="AJ5" s="47"/>
+      <c r="AK5" s="48">
         <v>44218</v>
       </c>
-      <c r="AL5" s="58"/>
-      <c r="AM5" s="57">
+      <c r="AL5" s="48"/>
+      <c r="AM5" s="47">
         <v>44225</v>
       </c>
-      <c r="AN5" s="57"/>
-      <c r="AO5" s="59">
+      <c r="AN5" s="47"/>
+      <c r="AO5" s="49">
         <v>44232</v>
       </c>
-      <c r="AP5" s="60"/>
-      <c r="AQ5" s="61">
+      <c r="AP5" s="43"/>
+      <c r="AQ5" s="44">
         <v>44239</v>
       </c>
-      <c r="AR5" s="61"/>
-      <c r="AS5" s="60">
+      <c r="AR5" s="44"/>
+      <c r="AS5" s="43">
         <v>44246</v>
       </c>
-      <c r="AT5" s="60"/>
-      <c r="AU5" s="61">
+      <c r="AT5" s="43"/>
+      <c r="AU5" s="44">
         <v>44253</v>
       </c>
-      <c r="AV5" s="61"/>
-      <c r="AW5" s="73">
+      <c r="AV5" s="44"/>
+      <c r="AW5" s="45">
         <v>44260</v>
       </c>
-      <c r="AX5" s="74"/>
-      <c r="AY5" s="69">
+      <c r="AX5" s="46"/>
+      <c r="AY5" s="39">
         <v>44267</v>
       </c>
-      <c r="AZ5" s="69"/>
-      <c r="BA5" s="74">
+      <c r="AZ5" s="39"/>
+      <c r="BA5" s="46">
         <v>44274</v>
       </c>
-      <c r="BB5" s="74"/>
-      <c r="BC5" s="69">
+      <c r="BB5" s="46"/>
+      <c r="BC5" s="39">
         <v>44281</v>
       </c>
-      <c r="BD5" s="70"/>
-      <c r="BE5" s="71">
+      <c r="BD5" s="40"/>
+      <c r="BE5" s="41">
         <v>44288</v>
       </c>
-      <c r="BF5" s="62"/>
-      <c r="BG5" s="72">
+      <c r="BF5" s="31"/>
+      <c r="BG5" s="42">
         <v>44295</v>
       </c>
-      <c r="BH5" s="72"/>
-      <c r="BI5" s="62">
+      <c r="BH5" s="42"/>
+      <c r="BI5" s="31">
         <v>44302</v>
       </c>
-      <c r="BJ5" s="62"/>
-      <c r="BK5" s="72">
+      <c r="BJ5" s="31"/>
+      <c r="BK5" s="42">
         <v>44309</v>
       </c>
-      <c r="BL5" s="72"/>
-      <c r="BM5" s="62">
+      <c r="BL5" s="42"/>
+      <c r="BM5" s="31">
         <v>44316</v>
       </c>
-      <c r="BN5" s="63"/>
+      <c r="BN5" s="32"/>
       <c r="BO5" s="16"/>
       <c r="BP5" s="6"/>
     </row>
     <row r="6" spans="2:68" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="68"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
       <c r="I6" s="21">
         <v>1</v>
       </c>
@@ -1802,10 +1802,10 @@
       </c>
     </row>
     <row r="7" spans="2:68" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="46"/>
+      <c r="C7" s="36"/>
       <c r="D7" s="4">
         <v>8</v>
       </c>
@@ -1825,10 +1825,10 @@
       <c r="J7" s="24"/>
     </row>
     <row r="8" spans="2:68" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="46"/>
+      <c r="C8" s="36"/>
       <c r="D8" s="4">
         <v>41</v>
       </c>
@@ -1844,10 +1844,10 @@
       <c r="J8" s="23"/>
     </row>
     <row r="9" spans="2:68" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="46"/>
+      <c r="C9" s="36"/>
       <c r="D9" s="4">
         <v>1</v>
       </c>
@@ -1863,10 +1863,10 @@
       <c r="J9" s="23"/>
     </row>
     <row r="10" spans="2:68" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="47"/>
+      <c r="C10" s="61"/>
       <c r="D10" s="29">
         <v>1</v>
       </c>
@@ -1978,10 +1978,10 @@
       <c r="J14" s="23"/>
     </row>
     <row r="15" spans="2:68" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="47" t="s">
+      <c r="B15" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="47"/>
+      <c r="C15" s="61"/>
       <c r="D15" s="29">
         <v>5</v>
       </c>
@@ -2162,10 +2162,10 @@
       <c r="J22" s="23"/>
     </row>
     <row r="23" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="47" t="s">
+      <c r="B23" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="47"/>
+      <c r="C23" s="61"/>
       <c r="D23" s="29">
         <v>19</v>
       </c>
@@ -2176,7 +2176,7 @@
         <v>27</v>
       </c>
       <c r="G23" s="29">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H23" s="30">
         <v>0</v>
@@ -2248,7 +2248,7 @@
         <v>1</v>
       </c>
       <c r="H26" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26" s="23"/>
       <c r="J26" s="23"/>
@@ -2264,8 +2264,12 @@
       <c r="E27" s="4">
         <v>1</v>
       </c>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
+      <c r="F27" s="4">
+        <v>42</v>
+      </c>
+      <c r="G27" s="4">
+        <v>1</v>
+      </c>
       <c r="H27" s="5">
         <v>0</v>
       </c>
@@ -2349,10 +2353,10 @@
       <c r="J31" s="23"/>
     </row>
     <row r="32" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="47" t="s">
+      <c r="B32" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="47"/>
+      <c r="C32" s="61"/>
       <c r="D32" s="29">
         <v>33</v>
       </c>
@@ -2425,10 +2429,10 @@
       <c r="J35" s="23"/>
     </row>
     <row r="36" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="41" t="s">
+      <c r="B36" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="C36" s="41"/>
+      <c r="C36" s="57"/>
       <c r="D36" s="29">
         <v>41</v>
       </c>
@@ -2502,6 +2506,40 @@
     </row>
   </sheetData>
   <mergeCells count="50">
+    <mergeCell ref="AJ2:AQ2"/>
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="AB2:AH2"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="AK5:AL5"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="AO5:AP5"/>
+    <mergeCell ref="AQ5:AR5"/>
     <mergeCell ref="BM5:BN5"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="G2:H2"/>
@@ -2518,40 +2556,6 @@
     <mergeCell ref="AW5:AX5"/>
     <mergeCell ref="AY5:AZ5"/>
     <mergeCell ref="BA5:BB5"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="AK5:AL5"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="AO5:AP5"/>
-    <mergeCell ref="AQ5:AR5"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="H4:H6"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="AJ2:AQ2"/>
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="AB2:AH2"/>
   </mergeCells>
   <conditionalFormatting sqref="I7:BP39">
     <cfRule type="expression" dxfId="9" priority="1">

</xml_diff>

<commit_message>
Moved foci operations into scg state and character context
</commit_message>
<xml_diff>
--- a/documentation/Interim Report/Gantt Chart.xlsx
+++ b/documentation/Interim Report/Gantt Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domin\Documents\University\CO3201\documentation\Interim Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBFA8B8B-A920-4F0E-A999-B91AB9006664}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C28E69B-CABD-4FBF-8DE1-B2278F5F5430}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -798,6 +798,99 @@
     <xf numFmtId="9" fontId="5" fillId="20" borderId="0" xfId="6" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="13" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="13" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="13" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="14" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="14" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="15" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="15" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="16" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="17" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="17" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="16" fontId="9" fillId="19" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -813,9 +906,6 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -834,101 +924,11 @@
     <xf numFmtId="16" fontId="13" fillId="19" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="9" fillId="17" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="16" fontId="9" fillId="18" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="16" fontId="9" fillId="18" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="16" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="17" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="15" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="15" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="14" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="14" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="13" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="13" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="13" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1341,8 +1341,8 @@
   </sheetPr>
   <dimension ref="B1:BP39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="AW14" sqref="AW14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D13" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="AM20" sqref="AM20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1368,62 +1368,62 @@
       <c r="H1" s="8"/>
     </row>
     <row r="2" spans="2:68" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="34" t="s">
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="35"/>
+      <c r="H2" s="66"/>
       <c r="I2" s="25">
         <v>57</v>
       </c>
       <c r="K2" s="9"/>
-      <c r="L2" s="67" t="s">
+      <c r="L2" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="68"/>
-      <c r="N2" s="68"/>
-      <c r="O2" s="68"/>
-      <c r="P2" s="69"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="35"/>
       <c r="Q2" s="10"/>
-      <c r="R2" s="67" t="s">
+      <c r="R2" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="70"/>
-      <c r="T2" s="70"/>
-      <c r="U2" s="69"/>
+      <c r="S2" s="36"/>
+      <c r="T2" s="36"/>
+      <c r="U2" s="35"/>
       <c r="V2" s="11"/>
-      <c r="W2" s="65" t="s">
+      <c r="W2" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="X2" s="66"/>
-      <c r="Y2" s="66"/>
-      <c r="Z2" s="71"/>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="32"/>
+      <c r="Z2" s="37"/>
       <c r="AA2" s="12"/>
-      <c r="AB2" s="72" t="s">
+      <c r="AB2" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="AC2" s="73"/>
-      <c r="AD2" s="73"/>
-      <c r="AE2" s="73"/>
-      <c r="AF2" s="73"/>
-      <c r="AG2" s="73"/>
-      <c r="AH2" s="74"/>
+      <c r="AC2" s="39"/>
+      <c r="AD2" s="39"/>
+      <c r="AE2" s="39"/>
+      <c r="AF2" s="39"/>
+      <c r="AG2" s="39"/>
+      <c r="AH2" s="40"/>
       <c r="AI2" s="13"/>
-      <c r="AJ2" s="65" t="s">
+      <c r="AJ2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="AK2" s="66"/>
-      <c r="AL2" s="66"/>
-      <c r="AM2" s="66"/>
-      <c r="AN2" s="66"/>
-      <c r="AO2" s="66"/>
-      <c r="AP2" s="66"/>
-      <c r="AQ2" s="66"/>
+      <c r="AK2" s="32"/>
+      <c r="AL2" s="32"/>
+      <c r="AM2" s="32"/>
+      <c r="AN2" s="32"/>
+      <c r="AO2" s="32"/>
+      <c r="AP2" s="32"/>
+      <c r="AQ2" s="32"/>
     </row>
     <row r="3" spans="2:68" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C3"/>
@@ -1454,23 +1454,23 @@
       <c r="AB3"/>
     </row>
     <row r="4" spans="2:68" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="62" t="s">
+      <c r="B4" s="67" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="67"/>
+      <c r="D4" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="62" t="s">
+      <c r="E4" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="62" t="s">
+      <c r="F4" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="62" t="s">
+      <c r="G4" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="64" t="s">
+      <c r="H4" s="50" t="s">
         <v>10</v>
       </c>
       <c r="I4" s="15" t="s">
@@ -1486,140 +1486,140 @@
       <c r="O4" s="14"/>
     </row>
     <row r="5" spans="2:68" s="7" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="64"/>
-      <c r="I5" s="58">
+      <c r="B5" s="67"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="42">
         <v>44120</v>
       </c>
-      <c r="J5" s="59"/>
-      <c r="K5" s="59">
+      <c r="J5" s="43"/>
+      <c r="K5" s="43">
         <v>44127</v>
       </c>
-      <c r="L5" s="60"/>
-      <c r="M5" s="54">
+      <c r="L5" s="44"/>
+      <c r="M5" s="45">
         <v>44134</v>
       </c>
-      <c r="N5" s="54"/>
-      <c r="O5" s="54">
+      <c r="N5" s="45"/>
+      <c r="O5" s="45">
         <v>44141</v>
       </c>
-      <c r="P5" s="54"/>
-      <c r="Q5" s="54">
+      <c r="P5" s="45"/>
+      <c r="Q5" s="45">
         <v>44148</v>
       </c>
-      <c r="R5" s="54"/>
-      <c r="S5" s="55">
+      <c r="R5" s="45"/>
+      <c r="S5" s="51">
         <v>44155</v>
       </c>
-      <c r="T5" s="55"/>
-      <c r="U5" s="54">
+      <c r="T5" s="51"/>
+      <c r="U5" s="45">
         <v>44162</v>
       </c>
-      <c r="V5" s="56"/>
-      <c r="W5" s="51">
+      <c r="V5" s="52"/>
+      <c r="W5" s="53">
         <v>44169</v>
       </c>
-      <c r="X5" s="51"/>
-      <c r="Y5" s="50">
+      <c r="X5" s="53"/>
+      <c r="Y5" s="54">
         <v>44176</v>
       </c>
-      <c r="Z5" s="50"/>
-      <c r="AA5" s="51">
+      <c r="Z5" s="54"/>
+      <c r="AA5" s="53">
         <v>44183</v>
       </c>
-      <c r="AB5" s="51"/>
-      <c r="AC5" s="50">
+      <c r="AB5" s="53"/>
+      <c r="AC5" s="54">
         <v>44190</v>
       </c>
-      <c r="AD5" s="52"/>
-      <c r="AE5" s="53">
+      <c r="AD5" s="55"/>
+      <c r="AE5" s="56">
         <v>44197</v>
       </c>
-      <c r="AF5" s="47"/>
-      <c r="AG5" s="48">
+      <c r="AF5" s="57"/>
+      <c r="AG5" s="58">
         <v>44204</v>
       </c>
-      <c r="AH5" s="48"/>
-      <c r="AI5" s="47">
+      <c r="AH5" s="58"/>
+      <c r="AI5" s="57">
         <v>44211</v>
       </c>
-      <c r="AJ5" s="47"/>
-      <c r="AK5" s="48">
+      <c r="AJ5" s="57"/>
+      <c r="AK5" s="58">
         <v>44218</v>
       </c>
-      <c r="AL5" s="48"/>
-      <c r="AM5" s="47">
+      <c r="AL5" s="58"/>
+      <c r="AM5" s="57">
         <v>44225</v>
       </c>
-      <c r="AN5" s="47"/>
-      <c r="AO5" s="49">
+      <c r="AN5" s="57"/>
+      <c r="AO5" s="59">
         <v>44232</v>
       </c>
-      <c r="AP5" s="43"/>
-      <c r="AQ5" s="44">
+      <c r="AP5" s="60"/>
+      <c r="AQ5" s="61">
         <v>44239</v>
       </c>
-      <c r="AR5" s="44"/>
-      <c r="AS5" s="43">
+      <c r="AR5" s="61"/>
+      <c r="AS5" s="60">
         <v>44246</v>
       </c>
-      <c r="AT5" s="43"/>
-      <c r="AU5" s="44">
+      <c r="AT5" s="60"/>
+      <c r="AU5" s="61">
         <v>44253</v>
       </c>
-      <c r="AV5" s="44"/>
-      <c r="AW5" s="45">
+      <c r="AV5" s="61"/>
+      <c r="AW5" s="73">
         <v>44260</v>
       </c>
-      <c r="AX5" s="46"/>
-      <c r="AY5" s="39">
+      <c r="AX5" s="74"/>
+      <c r="AY5" s="69">
         <v>44267</v>
       </c>
-      <c r="AZ5" s="39"/>
-      <c r="BA5" s="46">
+      <c r="AZ5" s="69"/>
+      <c r="BA5" s="74">
         <v>44274</v>
       </c>
-      <c r="BB5" s="46"/>
-      <c r="BC5" s="39">
+      <c r="BB5" s="74"/>
+      <c r="BC5" s="69">
         <v>44281</v>
       </c>
-      <c r="BD5" s="40"/>
-      <c r="BE5" s="41">
+      <c r="BD5" s="70"/>
+      <c r="BE5" s="71">
         <v>44288</v>
       </c>
-      <c r="BF5" s="31"/>
-      <c r="BG5" s="42">
+      <c r="BF5" s="62"/>
+      <c r="BG5" s="72">
         <v>44295</v>
       </c>
-      <c r="BH5" s="42"/>
-      <c r="BI5" s="31">
+      <c r="BH5" s="72"/>
+      <c r="BI5" s="62">
         <v>44302</v>
       </c>
-      <c r="BJ5" s="31"/>
-      <c r="BK5" s="42">
+      <c r="BJ5" s="62"/>
+      <c r="BK5" s="72">
         <v>44309</v>
       </c>
-      <c r="BL5" s="42"/>
-      <c r="BM5" s="31">
+      <c r="BL5" s="72"/>
+      <c r="BM5" s="62">
         <v>44316</v>
       </c>
-      <c r="BN5" s="32"/>
+      <c r="BN5" s="63"/>
       <c r="BO5" s="16"/>
       <c r="BP5" s="6"/>
     </row>
     <row r="6" spans="2:68" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="63"/>
-      <c r="H6" s="63"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
       <c r="I6" s="21">
         <v>1</v>
       </c>
@@ -1802,10 +1802,10 @@
       </c>
     </row>
     <row r="7" spans="2:68" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="36"/>
+      <c r="C7" s="46"/>
       <c r="D7" s="4">
         <v>8</v>
       </c>
@@ -1825,10 +1825,10 @@
       <c r="J7" s="24"/>
     </row>
     <row r="8" spans="2:68" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="36"/>
+      <c r="C8" s="46"/>
       <c r="D8" s="4">
         <v>41</v>
       </c>
@@ -1844,10 +1844,10 @@
       <c r="J8" s="23"/>
     </row>
     <row r="9" spans="2:68" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="36"/>
+      <c r="C9" s="46"/>
       <c r="D9" s="4">
         <v>1</v>
       </c>
@@ -1863,10 +1863,10 @@
       <c r="J9" s="23"/>
     </row>
     <row r="10" spans="2:68" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="61" t="s">
+      <c r="B10" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="61"/>
+      <c r="C10" s="47"/>
       <c r="D10" s="29">
         <v>1</v>
       </c>
@@ -1978,10 +1978,10 @@
       <c r="J14" s="23"/>
     </row>
     <row r="15" spans="2:68" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="61" t="s">
+      <c r="B15" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="61"/>
+      <c r="C15" s="47"/>
       <c r="D15" s="29">
         <v>5</v>
       </c>
@@ -2162,10 +2162,10 @@
       <c r="J22" s="23"/>
     </row>
     <row r="23" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="61" t="s">
+      <c r="B23" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="61"/>
+      <c r="C23" s="47"/>
       <c r="D23" s="29">
         <v>19</v>
       </c>
@@ -2176,7 +2176,7 @@
         <v>27</v>
       </c>
       <c r="G23" s="29">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="H23" s="30">
         <v>0</v>
@@ -2271,7 +2271,7 @@
         <v>1</v>
       </c>
       <c r="H27" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I27" s="23"/>
       <c r="J27" s="23"/>
@@ -2287,8 +2287,12 @@
       <c r="E28" s="4">
         <v>1</v>
       </c>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
+      <c r="F28" s="4">
+        <v>43</v>
+      </c>
+      <c r="G28" s="4">
+        <v>1</v>
+      </c>
       <c r="H28" s="5">
         <v>0</v>
       </c>
@@ -2353,10 +2357,10 @@
       <c r="J31" s="23"/>
     </row>
     <row r="32" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="61" t="s">
+      <c r="B32" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="61"/>
+      <c r="C32" s="47"/>
       <c r="D32" s="29">
         <v>33</v>
       </c>
@@ -2429,10 +2433,10 @@
       <c r="J35" s="23"/>
     </row>
     <row r="36" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="57" t="s">
+      <c r="B36" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="C36" s="57"/>
+      <c r="C36" s="41"/>
       <c r="D36" s="29">
         <v>41</v>
       </c>
@@ -2506,40 +2510,6 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="AJ2:AQ2"/>
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="AB2:AH2"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="H4:H6"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="AK5:AL5"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="AO5:AP5"/>
-    <mergeCell ref="AQ5:AR5"/>
     <mergeCell ref="BM5:BN5"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="G2:H2"/>
@@ -2556,6 +2526,40 @@
     <mergeCell ref="AW5:AX5"/>
     <mergeCell ref="AY5:AZ5"/>
     <mergeCell ref="BA5:BB5"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="AK5:AL5"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="AO5:AP5"/>
+    <mergeCell ref="AQ5:AR5"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="AJ2:AQ2"/>
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="AB2:AH2"/>
   </mergeCells>
   <conditionalFormatting sqref="I7:BP39">
     <cfRule type="expression" dxfId="9" priority="1">

</xml_diff>

<commit_message>
Psychic Panel functionality complete
</commit_message>
<xml_diff>
--- a/documentation/Interim Report/Gantt Chart.xlsx
+++ b/documentation/Interim Report/Gantt Chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domin\Documents\University\CO3201\documentation\Interim Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C28E69B-CABD-4FBF-8DE1-B2278F5F5430}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF455EC3-D61F-4081-9882-388B86945579}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25490" yWindow="-2940" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
   <si>
     <t>Project Planner</t>
   </si>
@@ -392,7 +392,7 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="21">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -509,6 +509,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -708,7 +714,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -728,9 +734,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -753,9 +756,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -798,6 +798,108 @@
     <xf numFmtId="9" fontId="5" fillId="20" borderId="0" xfId="6" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="9" fillId="19" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="19" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="12" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="19" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="19" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="17" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="18" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="18" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="16" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="17" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="15" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="15" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="14" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="14" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="13" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="13" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="13" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -828,107 +930,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="13" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="13" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="13" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="14" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="21" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="21" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="21" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="14" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="15" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="15" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="16" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="17" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="17" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="19" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="19" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="12" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="19" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="19" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="18" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="18" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1339,10 +1351,10 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:BP39"/>
+  <dimension ref="B1:BR40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D13" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="AM20" sqref="AM20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="R32" sqref="R32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1357,75 +1369,75 @@
     <col min="9" max="28" width="3.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:68" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="C1" s="27" t="s">
+    <row r="1" spans="2:70" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
+      <c r="C1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-    </row>
-    <row r="2" spans="2:68" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="64" t="s">
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+    </row>
+    <row r="2" spans="2:70" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="65" t="s">
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="66"/>
-      <c r="I2" s="25">
-        <v>57</v>
-      </c>
-      <c r="K2" s="9"/>
-      <c r="L2" s="33" t="s">
+      <c r="H2" s="33"/>
+      <c r="I2" s="23">
+        <v>60</v>
+      </c>
+      <c r="K2" s="8"/>
+      <c r="L2" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="33" t="s">
+      <c r="M2" s="66"/>
+      <c r="N2" s="66"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="67"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="36"/>
-      <c r="T2" s="36"/>
-      <c r="U2" s="35"/>
-      <c r="V2" s="11"/>
-      <c r="W2" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="X2" s="32"/>
-      <c r="Y2" s="32"/>
-      <c r="Z2" s="37"/>
-      <c r="AA2" s="12"/>
-      <c r="AB2" s="38" t="s">
+      <c r="S2" s="68"/>
+      <c r="T2" s="68"/>
+      <c r="U2" s="67"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="63" t="s">
+        <v>2</v>
+      </c>
+      <c r="X2" s="64"/>
+      <c r="Y2" s="64"/>
+      <c r="Z2" s="69"/>
+      <c r="AA2" s="11"/>
+      <c r="AB2" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="AC2" s="39"/>
-      <c r="AD2" s="39"/>
-      <c r="AE2" s="39"/>
-      <c r="AF2" s="39"/>
-      <c r="AG2" s="39"/>
-      <c r="AH2" s="40"/>
-      <c r="AI2" s="13"/>
-      <c r="AJ2" s="31" t="s">
+      <c r="AC2" s="71"/>
+      <c r="AD2" s="71"/>
+      <c r="AE2" s="71"/>
+      <c r="AF2" s="71"/>
+      <c r="AG2" s="71"/>
+      <c r="AH2" s="72"/>
+      <c r="AI2" s="12"/>
+      <c r="AJ2" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="AK2" s="32"/>
-      <c r="AL2" s="32"/>
-      <c r="AM2" s="32"/>
-      <c r="AN2" s="32"/>
-      <c r="AO2" s="32"/>
-      <c r="AP2" s="32"/>
-      <c r="AQ2" s="32"/>
-    </row>
-    <row r="3" spans="2:68" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="AK2" s="64"/>
+      <c r="AL2" s="64"/>
+      <c r="AM2" s="64"/>
+      <c r="AN2" s="64"/>
+      <c r="AO2" s="64"/>
+      <c r="AP2" s="64"/>
+      <c r="AQ2" s="64"/>
+    </row>
+    <row r="3" spans="2:70" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C3"/>
       <c r="D3"/>
       <c r="E3"/>
@@ -1453,359 +1465,365 @@
       <c r="AA3"/>
       <c r="AB3"/>
     </row>
-    <row r="4" spans="2:68" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="67" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="67"/>
-      <c r="D4" s="48" t="s">
+    <row r="4" spans="2:70" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="35"/>
+      <c r="D4" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="48" t="s">
+      <c r="E4" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="48" t="s">
+      <c r="F4" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="48" t="s">
+      <c r="G4" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="50" t="s">
+      <c r="H4" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="I4" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="15" t="s">
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-    </row>
-    <row r="5" spans="2:68" s="7" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="67"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="42">
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+    </row>
+    <row r="5" spans="2:70" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="56">
         <v>44120</v>
       </c>
-      <c r="J5" s="43"/>
-      <c r="K5" s="43">
+      <c r="J5" s="57"/>
+      <c r="K5" s="57">
         <v>44127</v>
       </c>
-      <c r="L5" s="44"/>
-      <c r="M5" s="45">
+      <c r="L5" s="58"/>
+      <c r="M5" s="52">
         <v>44134</v>
       </c>
-      <c r="N5" s="45"/>
-      <c r="O5" s="45">
+      <c r="N5" s="52"/>
+      <c r="O5" s="52">
         <v>44141</v>
       </c>
-      <c r="P5" s="45"/>
-      <c r="Q5" s="45">
+      <c r="P5" s="52"/>
+      <c r="Q5" s="52">
         <v>44148</v>
       </c>
-      <c r="R5" s="45"/>
-      <c r="S5" s="51">
+      <c r="R5" s="52"/>
+      <c r="S5" s="53">
         <v>44155</v>
       </c>
-      <c r="T5" s="51"/>
-      <c r="U5" s="45">
+      <c r="T5" s="53"/>
+      <c r="U5" s="52">
         <v>44162</v>
       </c>
-      <c r="V5" s="52"/>
-      <c r="W5" s="53">
+      <c r="V5" s="54"/>
+      <c r="W5" s="49">
         <v>44169</v>
       </c>
-      <c r="X5" s="53"/>
-      <c r="Y5" s="54">
+      <c r="X5" s="49"/>
+      <c r="Y5" s="48">
         <v>44176</v>
       </c>
-      <c r="Z5" s="54"/>
-      <c r="AA5" s="53">
+      <c r="Z5" s="48"/>
+      <c r="AA5" s="49">
         <v>44183</v>
       </c>
-      <c r="AB5" s="53"/>
-      <c r="AC5" s="54">
+      <c r="AB5" s="49"/>
+      <c r="AC5" s="48">
         <v>44190</v>
       </c>
-      <c r="AD5" s="55"/>
-      <c r="AE5" s="56">
+      <c r="AD5" s="50"/>
+      <c r="AE5" s="51">
         <v>44197</v>
       </c>
-      <c r="AF5" s="57"/>
-      <c r="AG5" s="58">
+      <c r="AF5" s="45"/>
+      <c r="AG5" s="46">
         <v>44204</v>
       </c>
-      <c r="AH5" s="58"/>
-      <c r="AI5" s="57">
+      <c r="AH5" s="46"/>
+      <c r="AI5" s="45">
         <v>44211</v>
       </c>
-      <c r="AJ5" s="57"/>
-      <c r="AK5" s="58">
+      <c r="AJ5" s="45"/>
+      <c r="AK5" s="46">
         <v>44218</v>
       </c>
-      <c r="AL5" s="58"/>
-      <c r="AM5" s="57">
+      <c r="AL5" s="46"/>
+      <c r="AM5" s="45">
         <v>44225</v>
       </c>
-      <c r="AN5" s="57"/>
-      <c r="AO5" s="59">
+      <c r="AN5" s="45"/>
+      <c r="AO5" s="47">
         <v>44232</v>
       </c>
-      <c r="AP5" s="60"/>
-      <c r="AQ5" s="61">
+      <c r="AP5" s="41"/>
+      <c r="AQ5" s="42">
         <v>44239</v>
       </c>
-      <c r="AR5" s="61"/>
-      <c r="AS5" s="60">
+      <c r="AR5" s="42"/>
+      <c r="AS5" s="41">
         <v>44246</v>
       </c>
-      <c r="AT5" s="60"/>
-      <c r="AU5" s="61">
+      <c r="AT5" s="41"/>
+      <c r="AU5" s="42">
         <v>44253</v>
       </c>
-      <c r="AV5" s="61"/>
-      <c r="AW5" s="73">
+      <c r="AV5" s="42"/>
+      <c r="AW5" s="43">
         <v>44260</v>
       </c>
-      <c r="AX5" s="74"/>
-      <c r="AY5" s="69">
+      <c r="AX5" s="44"/>
+      <c r="AY5" s="37">
         <v>44267</v>
       </c>
-      <c r="AZ5" s="69"/>
-      <c r="BA5" s="74">
+      <c r="AZ5" s="37"/>
+      <c r="BA5" s="44">
         <v>44274</v>
       </c>
-      <c r="BB5" s="74"/>
-      <c r="BC5" s="69">
+      <c r="BB5" s="44"/>
+      <c r="BC5" s="37">
         <v>44281</v>
       </c>
-      <c r="BD5" s="70"/>
-      <c r="BE5" s="71">
+      <c r="BD5" s="38"/>
+      <c r="BE5" s="39">
         <v>44288</v>
       </c>
-      <c r="BF5" s="62"/>
-      <c r="BG5" s="72">
+      <c r="BF5" s="29"/>
+      <c r="BG5" s="40">
         <v>44295</v>
       </c>
-      <c r="BH5" s="72"/>
-      <c r="BI5" s="62">
+      <c r="BH5" s="40"/>
+      <c r="BI5" s="29">
         <v>44302</v>
       </c>
-      <c r="BJ5" s="62"/>
-      <c r="BK5" s="72">
+      <c r="BJ5" s="29"/>
+      <c r="BK5" s="40">
         <v>44309</v>
       </c>
-      <c r="BL5" s="72"/>
-      <c r="BM5" s="62">
+      <c r="BL5" s="40"/>
+      <c r="BM5" s="29">
         <v>44316</v>
       </c>
-      <c r="BN5" s="63"/>
-      <c r="BO5" s="16"/>
-      <c r="BP5" s="6"/>
-    </row>
-    <row r="6" spans="2:68" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="68"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="21">
-        <v>1</v>
-      </c>
-      <c r="J6" s="21">
-        <v>2</v>
-      </c>
-      <c r="K6" s="21">
+      <c r="BN5" s="30"/>
+      <c r="BO5" s="73">
+        <v>44323</v>
+      </c>
+      <c r="BP5" s="74"/>
+      <c r="BQ5" s="75">
+        <v>44330</v>
+      </c>
+      <c r="BR5" s="76"/>
+    </row>
+    <row r="6" spans="2:70" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="61"/>
+      <c r="I6" s="19">
+        <v>1</v>
+      </c>
+      <c r="J6" s="19">
+        <v>2</v>
+      </c>
+      <c r="K6" s="19">
         <v>3</v>
       </c>
-      <c r="L6" s="21">
+      <c r="L6" s="19">
         <v>4</v>
       </c>
-      <c r="M6" s="22">
+      <c r="M6" s="20">
         <v>5</v>
       </c>
-      <c r="N6" s="22">
+      <c r="N6" s="20">
         <v>6</v>
       </c>
-      <c r="O6" s="22">
+      <c r="O6" s="20">
         <v>7</v>
       </c>
-      <c r="P6" s="22">
+      <c r="P6" s="20">
         <v>8</v>
       </c>
-      <c r="Q6" s="21">
+      <c r="Q6" s="19">
         <v>9</v>
       </c>
-      <c r="R6" s="21">
+      <c r="R6" s="19">
         <v>10</v>
       </c>
-      <c r="S6" s="21">
+      <c r="S6" s="19">
         <v>11</v>
       </c>
-      <c r="T6" s="21">
+      <c r="T6" s="19">
         <v>12</v>
       </c>
-      <c r="U6" s="22">
+      <c r="U6" s="20">
         <v>13</v>
       </c>
-      <c r="V6" s="22">
+      <c r="V6" s="20">
         <v>14</v>
       </c>
-      <c r="W6" s="22">
+      <c r="W6" s="20">
         <v>15</v>
       </c>
-      <c r="X6" s="22">
+      <c r="X6" s="20">
         <v>16</v>
       </c>
-      <c r="Y6" s="21">
+      <c r="Y6" s="19">
         <v>17</v>
       </c>
-      <c r="Z6" s="21">
+      <c r="Z6" s="19">
         <v>18</v>
       </c>
-      <c r="AA6" s="21">
+      <c r="AA6" s="19">
         <v>19</v>
       </c>
-      <c r="AB6" s="21">
+      <c r="AB6" s="19">
         <v>20</v>
       </c>
-      <c r="AC6" s="22">
+      <c r="AC6" s="20">
         <v>21</v>
       </c>
-      <c r="AD6" s="22">
+      <c r="AD6" s="20">
         <v>22</v>
       </c>
-      <c r="AE6" s="22">
+      <c r="AE6" s="20">
         <v>23</v>
       </c>
-      <c r="AF6" s="22">
+      <c r="AF6" s="20">
         <v>24</v>
       </c>
-      <c r="AG6" s="21">
+      <c r="AG6" s="19">
         <v>25</v>
       </c>
-      <c r="AH6" s="21">
+      <c r="AH6" s="19">
         <v>26</v>
       </c>
-      <c r="AI6" s="21">
+      <c r="AI6" s="19">
         <v>27</v>
       </c>
-      <c r="AJ6" s="21">
+      <c r="AJ6" s="19">
         <v>28</v>
       </c>
-      <c r="AK6" s="22">
+      <c r="AK6" s="20">
         <v>29</v>
       </c>
-      <c r="AL6" s="22">
+      <c r="AL6" s="20">
         <v>30</v>
       </c>
-      <c r="AM6" s="22">
+      <c r="AM6" s="20">
         <v>31</v>
       </c>
-      <c r="AN6" s="22">
+      <c r="AN6" s="20">
         <v>32</v>
       </c>
-      <c r="AO6" s="21">
+      <c r="AO6" s="19">
         <v>33</v>
       </c>
-      <c r="AP6" s="21">
+      <c r="AP6" s="19">
         <v>34</v>
       </c>
-      <c r="AQ6" s="21">
+      <c r="AQ6" s="19">
         <v>35</v>
       </c>
-      <c r="AR6" s="21">
+      <c r="AR6" s="19">
         <v>36</v>
       </c>
-      <c r="AS6" s="22">
+      <c r="AS6" s="20">
         <v>37</v>
       </c>
-      <c r="AT6" s="22">
+      <c r="AT6" s="20">
         <v>38</v>
       </c>
-      <c r="AU6" s="22">
+      <c r="AU6" s="20">
         <v>39</v>
       </c>
-      <c r="AV6" s="22">
+      <c r="AV6" s="20">
         <v>40</v>
       </c>
-      <c r="AW6" s="21">
+      <c r="AW6" s="19">
         <v>41</v>
       </c>
-      <c r="AX6" s="21">
+      <c r="AX6" s="19">
         <v>42</v>
       </c>
-      <c r="AY6" s="21">
+      <c r="AY6" s="19">
         <v>43</v>
       </c>
-      <c r="AZ6" s="21">
+      <c r="AZ6" s="19">
         <v>44</v>
       </c>
-      <c r="BA6" s="22">
+      <c r="BA6" s="20">
         <v>45</v>
       </c>
-      <c r="BB6" s="22">
+      <c r="BB6" s="20">
         <v>46</v>
       </c>
-      <c r="BC6" s="22">
+      <c r="BC6" s="20">
         <v>47</v>
       </c>
-      <c r="BD6" s="22">
+      <c r="BD6" s="20">
         <v>48</v>
       </c>
-      <c r="BE6" s="21">
+      <c r="BE6" s="19">
         <v>49</v>
       </c>
-      <c r="BF6" s="21">
+      <c r="BF6" s="19">
         <v>50</v>
       </c>
-      <c r="BG6" s="21">
+      <c r="BG6" s="19">
         <v>51</v>
       </c>
-      <c r="BH6" s="21">
+      <c r="BH6" s="19">
         <v>52</v>
       </c>
-      <c r="BI6" s="22">
+      <c r="BI6" s="20">
         <v>53</v>
       </c>
-      <c r="BJ6" s="22">
+      <c r="BJ6" s="20">
         <v>54</v>
       </c>
-      <c r="BK6" s="22">
+      <c r="BK6" s="20">
         <v>55</v>
       </c>
-      <c r="BL6" s="22">
+      <c r="BL6" s="20">
         <v>56</v>
       </c>
-      <c r="BM6" s="21">
+      <c r="BM6" s="19">
         <v>57</v>
       </c>
-      <c r="BN6" s="21">
+      <c r="BN6" s="19">
         <v>58</v>
       </c>
-      <c r="BO6" s="21">
+      <c r="BO6" s="19">
         <v>59</v>
       </c>
-      <c r="BP6" s="21">
+      <c r="BP6" s="19">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="2:68" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="46" t="s">
+    <row r="7" spans="2:70" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="46"/>
+      <c r="C7" s="34"/>
       <c r="D7" s="4">
         <v>8</v>
       </c>
@@ -1821,73 +1839,81 @@
       <c r="H7" s="5">
         <v>1</v>
       </c>
-      <c r="I7" s="23"/>
-      <c r="J7" s="24"/>
-    </row>
-    <row r="8" spans="2:68" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="46" t="s">
+      <c r="I7" s="21"/>
+      <c r="J7" s="22"/>
+    </row>
+    <row r="8" spans="2:70" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="46"/>
+      <c r="C8" s="34"/>
       <c r="D8" s="4">
         <v>41</v>
       </c>
       <c r="E8" s="4">
         <v>16</v>
       </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="F8" s="4">
+        <v>59</v>
+      </c>
+      <c r="G8" s="4">
+        <v>2</v>
+      </c>
       <c r="H8" s="5">
         <v>0</v>
       </c>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-    </row>
-    <row r="9" spans="2:68" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="46" t="s">
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+    </row>
+    <row r="9" spans="2:70" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="46"/>
+      <c r="C9" s="34"/>
       <c r="D9" s="4">
         <v>1</v>
       </c>
       <c r="E9" s="4">
         <v>56</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="F9" s="4">
+        <v>1</v>
+      </c>
+      <c r="G9" s="4">
+        <v>59</v>
+      </c>
       <c r="H9" s="5">
-        <v>0</v>
-      </c>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-    </row>
-    <row r="10" spans="2:68" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="47" t="s">
+        <v>0.8</v>
+      </c>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+    </row>
+    <row r="10" spans="2:70" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="47"/>
-      <c r="D10" s="29">
-        <v>1</v>
-      </c>
-      <c r="E10" s="29">
+      <c r="C10" s="59"/>
+      <c r="D10" s="27">
+        <v>1</v>
+      </c>
+      <c r="E10" s="27">
         <v>4</v>
       </c>
-      <c r="F10" s="29">
-        <v>1</v>
-      </c>
-      <c r="G10" s="29">
+      <c r="F10" s="27">
+        <v>1</v>
+      </c>
+      <c r="G10" s="27">
         <v>4</v>
       </c>
-      <c r="H10" s="30">
-        <v>1</v>
-      </c>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
-    </row>
-    <row r="11" spans="2:68" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="18"/>
-      <c r="C11" s="17" t="s">
+      <c r="H10" s="28">
+        <v>1</v>
+      </c>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+    </row>
+    <row r="11" spans="2:70" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="16"/>
+      <c r="C11" s="15" t="s">
         <v>15</v>
       </c>
       <c r="D11" s="4">
@@ -1905,12 +1931,12 @@
       <c r="H11" s="5">
         <v>1</v>
       </c>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
-    </row>
-    <row r="12" spans="2:68" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="18"/>
-      <c r="C12" s="17" t="s">
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
+    </row>
+    <row r="12" spans="2:70" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="16"/>
+      <c r="C12" s="15" t="s">
         <v>22</v>
       </c>
       <c r="D12" s="4">
@@ -1928,12 +1954,12 @@
       <c r="H12" s="5">
         <v>1</v>
       </c>
-      <c r="I12" s="23"/>
-      <c r="J12" s="23"/>
-    </row>
-    <row r="13" spans="2:68" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="18"/>
-      <c r="C13" s="17" t="s">
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+    </row>
+    <row r="13" spans="2:70" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="16"/>
+      <c r="C13" s="15" t="s">
         <v>16</v>
       </c>
       <c r="D13" s="4">
@@ -1951,11 +1977,11 @@
       <c r="H13" s="5">
         <v>1</v>
       </c>
-      <c r="I13" s="23"/>
-      <c r="J13" s="23"/>
-    </row>
-    <row r="14" spans="2:68" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="18"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+    </row>
+    <row r="14" spans="2:70" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="16"/>
       <c r="C14" s="2" t="s">
         <v>17</v>
       </c>
@@ -1974,35 +2000,35 @@
       <c r="H14" s="5">
         <v>1</v>
       </c>
-      <c r="I14" s="23"/>
-      <c r="J14" s="23"/>
-    </row>
-    <row r="15" spans="2:68" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="47" t="s">
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+    </row>
+    <row r="15" spans="2:70" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="47"/>
-      <c r="D15" s="29">
+      <c r="C15" s="59"/>
+      <c r="D15" s="27">
         <v>5</v>
       </c>
-      <c r="E15" s="29">
+      <c r="E15" s="27">
         <v>14</v>
       </c>
-      <c r="F15" s="29">
+      <c r="F15" s="27">
         <v>5</v>
       </c>
-      <c r="G15" s="29">
+      <c r="G15" s="27">
         <v>22</v>
       </c>
-      <c r="H15" s="30">
-        <v>1</v>
-      </c>
-      <c r="I15" s="23"/>
-      <c r="J15" s="23"/>
-    </row>
-    <row r="16" spans="2:68" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="18"/>
-      <c r="C16" s="17" t="s">
+      <c r="H15" s="28">
+        <v>1</v>
+      </c>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
+    </row>
+    <row r="16" spans="2:70" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="16"/>
+      <c r="C16" s="15" t="s">
         <v>25</v>
       </c>
       <c r="D16" s="4">
@@ -2020,12 +2046,12 @@
       <c r="H16" s="5">
         <v>1</v>
       </c>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
     </row>
     <row r="17" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="18"/>
-      <c r="C17" s="17" t="s">
+      <c r="B17" s="16"/>
+      <c r="C17" s="15" t="s">
         <v>26</v>
       </c>
       <c r="D17" s="4">
@@ -2043,12 +2069,12 @@
       <c r="H17" s="5">
         <v>1</v>
       </c>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
     </row>
     <row r="18" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="18"/>
-      <c r="C18" s="17" t="s">
+      <c r="B18" s="16"/>
+      <c r="C18" s="15" t="s">
         <v>27</v>
       </c>
       <c r="D18" s="4">
@@ -2066,12 +2092,12 @@
       <c r="H18" s="5">
         <v>1</v>
       </c>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
     </row>
     <row r="19" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="18"/>
-      <c r="C19" s="17" t="s">
+      <c r="B19" s="16"/>
+      <c r="C19" s="15" t="s">
         <v>28</v>
       </c>
       <c r="D19" s="4">
@@ -2089,12 +2115,12 @@
       <c r="H19" s="5">
         <v>1</v>
       </c>
-      <c r="I19" s="23"/>
-      <c r="J19" s="23"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
     </row>
     <row r="20" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="18"/>
-      <c r="C20" s="17" t="s">
+      <c r="B20" s="16"/>
+      <c r="C20" s="15" t="s">
         <v>29</v>
       </c>
       <c r="D20" s="4">
@@ -2112,12 +2138,12 @@
       <c r="H20" s="5">
         <v>1</v>
       </c>
-      <c r="I20" s="23"/>
-      <c r="J20" s="23"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
     </row>
     <row r="21" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="18"/>
-      <c r="C21" s="17" t="s">
+      <c r="B21" s="16"/>
+      <c r="C21" s="15" t="s">
         <v>30</v>
       </c>
       <c r="D21" s="4">
@@ -2135,12 +2161,12 @@
       <c r="H21" s="5">
         <v>1</v>
       </c>
-      <c r="I21" s="23"/>
-      <c r="J21" s="23"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
     </row>
     <row r="22" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="18"/>
-      <c r="C22" s="17" t="s">
+      <c r="B22" s="16"/>
+      <c r="C22" s="15" t="s">
         <v>42</v>
       </c>
       <c r="D22" s="4">
@@ -2158,35 +2184,35 @@
       <c r="H22" s="5">
         <v>1</v>
       </c>
-      <c r="I22" s="23"/>
-      <c r="J22" s="23"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="21"/>
     </row>
     <row r="23" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="47" t="s">
+      <c r="B23" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="47"/>
-      <c r="D23" s="29">
+      <c r="C23" s="59"/>
+      <c r="D23" s="27">
         <v>19</v>
       </c>
-      <c r="E23" s="29">
+      <c r="E23" s="27">
         <v>14</v>
       </c>
-      <c r="F23" s="29">
+      <c r="F23" s="27">
         <v>27</v>
       </c>
-      <c r="G23" s="29">
+      <c r="G23" s="27">
         <v>20</v>
       </c>
-      <c r="H23" s="30">
+      <c r="H23" s="28">
         <v>0</v>
       </c>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21"/>
     </row>
     <row r="24" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="20"/>
-      <c r="C24" s="17" t="s">
+      <c r="B24" s="18"/>
+      <c r="C24" s="15" t="s">
         <v>25</v>
       </c>
       <c r="D24" s="4">
@@ -2204,12 +2230,12 @@
       <c r="H24" s="5">
         <v>1</v>
       </c>
-      <c r="I24" s="23"/>
-      <c r="J24" s="23"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
     </row>
     <row r="25" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="20"/>
-      <c r="C25" s="17" t="s">
+      <c r="B25" s="18"/>
+      <c r="C25" s="15" t="s">
         <v>26</v>
       </c>
       <c r="D25" s="4">
@@ -2227,12 +2253,12 @@
       <c r="H25" s="5">
         <v>1</v>
       </c>
-      <c r="I25" s="23"/>
-      <c r="J25" s="23"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
     </row>
     <row r="26" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="20"/>
-      <c r="C26" s="17" t="s">
+      <c r="B26" s="18"/>
+      <c r="C26" s="15" t="s">
         <v>27</v>
       </c>
       <c r="D26" s="4">
@@ -2250,12 +2276,12 @@
       <c r="H26" s="5">
         <v>1</v>
       </c>
-      <c r="I26" s="23"/>
-      <c r="J26" s="23"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="21"/>
     </row>
     <row r="27" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="20"/>
-      <c r="C27" s="17" t="s">
+      <c r="B27" s="18"/>
+      <c r="C27" s="15" t="s">
         <v>28</v>
       </c>
       <c r="D27" s="4">
@@ -2273,12 +2299,12 @@
       <c r="H27" s="5">
         <v>1</v>
       </c>
-      <c r="I27" s="23"/>
-      <c r="J27" s="23"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
     </row>
     <row r="28" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="20"/>
-      <c r="C28" s="17" t="s">
+      <c r="B28" s="18"/>
+      <c r="C28" s="15" t="s">
         <v>29</v>
       </c>
       <c r="D28" s="4">
@@ -2291,17 +2317,17 @@
         <v>43</v>
       </c>
       <c r="G28" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H28" s="5">
-        <v>0</v>
-      </c>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23"/>
+        <v>1</v>
+      </c>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21"/>
     </row>
     <row r="29" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="20"/>
-      <c r="C29" s="17" t="s">
+      <c r="B29" s="18"/>
+      <c r="C29" s="15" t="s">
         <v>30</v>
       </c>
       <c r="D29" s="4">
@@ -2310,97 +2336,113 @@
       <c r="E29" s="4">
         <v>2</v>
       </c>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
+      <c r="F29" s="4">
+        <v>51</v>
+      </c>
+      <c r="G29" s="4">
+        <v>2</v>
+      </c>
       <c r="H29" s="5">
-        <v>0</v>
-      </c>
-      <c r="I29" s="23"/>
-      <c r="J29" s="23"/>
+        <v>1</v>
+      </c>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
     </row>
     <row r="30" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="20"/>
-      <c r="C30" s="17" t="s">
+      <c r="B30" s="18"/>
+      <c r="C30" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" s="4">
+        <v>27</v>
+      </c>
+      <c r="E30" s="4">
+        <v>1</v>
+      </c>
+      <c r="F30" s="4">
+        <v>52</v>
+      </c>
+      <c r="G30" s="4">
+        <v>2</v>
+      </c>
+      <c r="H30" s="5">
+        <v>1</v>
+      </c>
+      <c r="I30" s="21"/>
+      <c r="J30" s="21"/>
+    </row>
+    <row r="31" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="18"/>
+      <c r="C31" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D31" s="4">
         <v>28</v>
       </c>
-      <c r="E30" s="4">
-        <v>2</v>
-      </c>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="5">
-        <v>0</v>
-      </c>
-      <c r="I30" s="23"/>
-      <c r="J30" s="23"/>
-    </row>
-    <row r="31" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="20"/>
-      <c r="C31" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="D31" s="4">
-        <v>30</v>
-      </c>
       <c r="E31" s="4">
-        <v>3</v>
-      </c>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
+        <v>2</v>
+      </c>
+      <c r="F31" s="4">
+        <v>56</v>
+      </c>
+      <c r="G31" s="4">
+        <v>2</v>
+      </c>
       <c r="H31" s="5">
         <v>0</v>
       </c>
-      <c r="I31" s="23"/>
-      <c r="J31" s="23"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21"/>
     </row>
     <row r="32" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="47" t="s">
+      <c r="B32" s="18"/>
+      <c r="C32" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" s="4">
+        <v>30</v>
+      </c>
+      <c r="E32" s="4">
+        <v>3</v>
+      </c>
+      <c r="F32" s="4">
+        <v>54</v>
+      </c>
+      <c r="G32" s="4">
+        <v>2</v>
+      </c>
+      <c r="H32" s="5">
+        <v>0</v>
+      </c>
+      <c r="I32" s="21"/>
+      <c r="J32" s="21"/>
+    </row>
+    <row r="33" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="47"/>
-      <c r="D32" s="29">
+      <c r="C33" s="59"/>
+      <c r="D33" s="27">
         <v>33</v>
       </c>
-      <c r="E32" s="29">
+      <c r="E33" s="27">
         <v>8</v>
       </c>
-      <c r="F32" s="29"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="30">
+      <c r="F33" s="27"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="28">
         <v>0</v>
       </c>
-      <c r="I32" s="23"/>
-      <c r="J32" s="23"/>
-    </row>
-    <row r="33" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="20"/>
-      <c r="C33" s="17" t="s">
+      <c r="I33" s="21"/>
+      <c r="J33" s="21"/>
+    </row>
+    <row r="34" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="18"/>
+      <c r="C34" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D33" s="4">
+      <c r="D34" s="4">
         <v>33</v>
-      </c>
-      <c r="E33" s="4">
-        <v>2</v>
-      </c>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="5">
-        <v>0</v>
-      </c>
-      <c r="I33" s="23"/>
-      <c r="J33" s="23"/>
-    </row>
-    <row r="34" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="20"/>
-      <c r="C34" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D34" s="4">
-        <v>35</v>
       </c>
       <c r="E34" s="4">
         <v>2</v>
@@ -2410,106 +2452,165 @@
       <c r="H34" s="5">
         <v>0</v>
       </c>
-      <c r="I34" s="23"/>
-      <c r="J34" s="23"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="21"/>
     </row>
     <row r="35" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="20"/>
-      <c r="C35" s="17" t="s">
-        <v>36</v>
+      <c r="B35" s="18"/>
+      <c r="C35" s="15" t="s">
+        <v>34</v>
       </c>
       <c r="D35" s="4">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E35" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
       <c r="H35" s="5">
         <v>0</v>
       </c>
-      <c r="I35" s="23"/>
-      <c r="J35" s="23"/>
+      <c r="I35" s="21"/>
+      <c r="J35" s="21"/>
     </row>
     <row r="36" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="41" t="s">
+      <c r="B36" s="18"/>
+      <c r="C36" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D36" s="4">
+        <v>37</v>
+      </c>
+      <c r="E36" s="4">
+        <v>4</v>
+      </c>
+      <c r="F36" s="4">
+        <v>58</v>
+      </c>
+      <c r="G36" s="4">
+        <v>2</v>
+      </c>
+      <c r="H36" s="5">
+        <v>0</v>
+      </c>
+      <c r="I36" s="21"/>
+      <c r="J36" s="21"/>
+    </row>
+    <row r="37" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="C36" s="41"/>
-      <c r="D36" s="29">
+      <c r="C37" s="55"/>
+      <c r="D37" s="27">
         <v>41</v>
       </c>
-      <c r="E36" s="29">
+      <c r="E37" s="27">
         <v>8</v>
       </c>
-      <c r="F36" s="29"/>
-      <c r="G36" s="29"/>
-      <c r="H36" s="30">
+      <c r="F37" s="27"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="28">
         <v>0</v>
       </c>
-      <c r="I36" s="23"/>
-      <c r="J36" s="23"/>
-    </row>
-    <row r="37" spans="2:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="26"/>
-      <c r="C37" s="19" t="s">
+      <c r="I37" s="21"/>
+      <c r="J37" s="21"/>
+    </row>
+    <row r="38" spans="2:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="24"/>
+      <c r="C38" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D37" s="4">
+      <c r="D38" s="4">
         <v>41</v>
       </c>
-      <c r="E37" s="4">
-        <v>2</v>
-      </c>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="5">
-        <v>0</v>
-      </c>
-      <c r="I37" s="23"/>
-      <c r="J37" s="23"/>
-    </row>
-    <row r="38" spans="2:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="26"/>
-      <c r="C38" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="D38" s="4">
-        <v>43</v>
-      </c>
       <c r="E38" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
       <c r="H38" s="5">
         <v>0</v>
       </c>
-      <c r="I38" s="23"/>
-      <c r="J38" s="23"/>
+      <c r="I38" s="21"/>
+      <c r="J38" s="21"/>
     </row>
     <row r="39" spans="2:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="28"/>
-      <c r="C39" s="19" t="s">
-        <v>39</v>
+      <c r="B39" s="24"/>
+      <c r="C39" s="17" t="s">
+        <v>38</v>
       </c>
       <c r="D39" s="4">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E39" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
       <c r="H39" s="5">
         <v>0</v>
       </c>
-      <c r="I39" s="23"/>
-      <c r="J39" s="23"/>
+      <c r="I39" s="21"/>
+      <c r="J39" s="21"/>
+    </row>
+    <row r="40" spans="2:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="26"/>
+      <c r="C40" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D40" s="4">
+        <v>47</v>
+      </c>
+      <c r="E40" s="4">
+        <v>2</v>
+      </c>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="5">
+        <v>0</v>
+      </c>
+      <c r="I40" s="21"/>
+      <c r="J40" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="50">
+  <mergeCells count="52">
+    <mergeCell ref="BO5:BP5"/>
+    <mergeCell ref="BQ5:BR5"/>
+    <mergeCell ref="AJ2:AQ2"/>
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="AB2:AH2"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="AK5:AL5"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="AO5:AP5"/>
+    <mergeCell ref="AQ5:AR5"/>
     <mergeCell ref="BM5:BN5"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="G2:H2"/>
@@ -2526,42 +2627,8 @@
     <mergeCell ref="AW5:AX5"/>
     <mergeCell ref="AY5:AZ5"/>
     <mergeCell ref="BA5:BB5"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="AK5:AL5"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="AO5:AP5"/>
-    <mergeCell ref="AQ5:AR5"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="H4:H6"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="AJ2:AQ2"/>
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="AB2:AH2"/>
   </mergeCells>
-  <conditionalFormatting sqref="I7:BP39">
+  <conditionalFormatting sqref="I7:BP40">
     <cfRule type="expression" dxfId="9" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -2587,7 +2654,7 @@
       <formula>MOD(ROUNDUP(COLUMN()/2,0),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C40:BP40">
+  <conditionalFormatting sqref="C41:BP41">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>TRUE</formula>
     </cfRule>

</xml_diff>

<commit_message>
Added selectors to EquipmentPackageAvatar and credits display to panel
</commit_message>
<xml_diff>
--- a/documentation/Interim Report/Gantt Chart.xlsx
+++ b/documentation/Interim Report/Gantt Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domin\Documents\University\CO3201\documentation\Interim Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF455EC3-D61F-4081-9882-388B86945579}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D00869-B78F-45C6-B756-9C4ED9D718C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25490" yWindow="-2940" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -798,6 +798,111 @@
     <xf numFmtId="9" fontId="5" fillId="20" borderId="0" xfId="6" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="21" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="21" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="21" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="13" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="13" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="13" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="14" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="14" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="15" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="15" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="16" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="17" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="17" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="16" fontId="9" fillId="19" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -813,9 +918,6 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -834,113 +936,11 @@
     <xf numFmtId="16" fontId="13" fillId="19" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="9" fillId="17" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="16" fontId="9" fillId="18" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="16" fontId="9" fillId="18" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="16" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="17" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="15" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="15" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="14" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="14" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="13" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="13" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="13" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="21" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="21" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="21" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1354,7 +1354,7 @@
   <dimension ref="B1:BR40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="R32" sqref="R32"/>
+      <selection activeCell="S31" sqref="S31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1380,62 +1380,62 @@
       <c r="H1" s="7"/>
     </row>
     <row r="2" spans="2:70" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="32" t="s">
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="33"/>
+      <c r="H2" s="68"/>
       <c r="I2" s="23">
         <v>60</v>
       </c>
       <c r="K2" s="8"/>
-      <c r="L2" s="65" t="s">
+      <c r="L2" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="66"/>
-      <c r="N2" s="66"/>
-      <c r="O2" s="66"/>
-      <c r="P2" s="67"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="37"/>
       <c r="Q2" s="9"/>
-      <c r="R2" s="65" t="s">
+      <c r="R2" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="68"/>
-      <c r="T2" s="68"/>
-      <c r="U2" s="67"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="37"/>
       <c r="V2" s="10"/>
-      <c r="W2" s="63" t="s">
+      <c r="W2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="X2" s="64"/>
-      <c r="Y2" s="64"/>
-      <c r="Z2" s="69"/>
+      <c r="X2" s="34"/>
+      <c r="Y2" s="34"/>
+      <c r="Z2" s="39"/>
       <c r="AA2" s="11"/>
-      <c r="AB2" s="70" t="s">
+      <c r="AB2" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="AC2" s="71"/>
-      <c r="AD2" s="71"/>
-      <c r="AE2" s="71"/>
-      <c r="AF2" s="71"/>
-      <c r="AG2" s="71"/>
-      <c r="AH2" s="72"/>
+      <c r="AC2" s="41"/>
+      <c r="AD2" s="41"/>
+      <c r="AE2" s="41"/>
+      <c r="AF2" s="41"/>
+      <c r="AG2" s="41"/>
+      <c r="AH2" s="42"/>
       <c r="AI2" s="12"/>
-      <c r="AJ2" s="63" t="s">
+      <c r="AJ2" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="AK2" s="64"/>
-      <c r="AL2" s="64"/>
-      <c r="AM2" s="64"/>
-      <c r="AN2" s="64"/>
-      <c r="AO2" s="64"/>
-      <c r="AP2" s="64"/>
-      <c r="AQ2" s="64"/>
+      <c r="AK2" s="34"/>
+      <c r="AL2" s="34"/>
+      <c r="AM2" s="34"/>
+      <c r="AN2" s="34"/>
+      <c r="AO2" s="34"/>
+      <c r="AP2" s="34"/>
+      <c r="AQ2" s="34"/>
     </row>
     <row r="3" spans="2:70" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C3"/>
@@ -1466,23 +1466,23 @@
       <c r="AB3"/>
     </row>
     <row r="4" spans="2:70" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="60" t="s">
+      <c r="B4" s="69" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="69"/>
+      <c r="D4" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="60" t="s">
+      <c r="E4" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="60" t="s">
+      <c r="F4" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="60" t="s">
+      <c r="G4" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="62" t="s">
+      <c r="H4" s="52" t="s">
         <v>10</v>
       </c>
       <c r="I4" s="14" t="s">
@@ -1498,146 +1498,146 @@
       <c r="O4" s="13"/>
     </row>
     <row r="5" spans="2:70" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
-      <c r="H5" s="62"/>
-      <c r="I5" s="56">
+      <c r="B5" s="69"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="44">
         <v>44120</v>
       </c>
-      <c r="J5" s="57"/>
-      <c r="K5" s="57">
+      <c r="J5" s="45"/>
+      <c r="K5" s="45">
         <v>44127</v>
       </c>
-      <c r="L5" s="58"/>
-      <c r="M5" s="52">
+      <c r="L5" s="46"/>
+      <c r="M5" s="47">
         <v>44134</v>
       </c>
-      <c r="N5" s="52"/>
-      <c r="O5" s="52">
+      <c r="N5" s="47"/>
+      <c r="O5" s="47">
         <v>44141</v>
       </c>
-      <c r="P5" s="52"/>
-      <c r="Q5" s="52">
+      <c r="P5" s="47"/>
+      <c r="Q5" s="47">
         <v>44148</v>
       </c>
-      <c r="R5" s="52"/>
+      <c r="R5" s="47"/>
       <c r="S5" s="53">
         <v>44155</v>
       </c>
       <c r="T5" s="53"/>
-      <c r="U5" s="52">
+      <c r="U5" s="47">
         <v>44162</v>
       </c>
       <c r="V5" s="54"/>
-      <c r="W5" s="49">
+      <c r="W5" s="55">
         <v>44169</v>
       </c>
-      <c r="X5" s="49"/>
-      <c r="Y5" s="48">
+      <c r="X5" s="55"/>
+      <c r="Y5" s="56">
         <v>44176</v>
       </c>
-      <c r="Z5" s="48"/>
-      <c r="AA5" s="49">
+      <c r="Z5" s="56"/>
+      <c r="AA5" s="55">
         <v>44183</v>
       </c>
-      <c r="AB5" s="49"/>
-      <c r="AC5" s="48">
+      <c r="AB5" s="55"/>
+      <c r="AC5" s="56">
         <v>44190</v>
       </c>
-      <c r="AD5" s="50"/>
-      <c r="AE5" s="51">
+      <c r="AD5" s="57"/>
+      <c r="AE5" s="58">
         <v>44197</v>
       </c>
-      <c r="AF5" s="45"/>
-      <c r="AG5" s="46">
+      <c r="AF5" s="59"/>
+      <c r="AG5" s="60">
         <v>44204</v>
       </c>
-      <c r="AH5" s="46"/>
-      <c r="AI5" s="45">
+      <c r="AH5" s="60"/>
+      <c r="AI5" s="59">
         <v>44211</v>
       </c>
-      <c r="AJ5" s="45"/>
-      <c r="AK5" s="46">
+      <c r="AJ5" s="59"/>
+      <c r="AK5" s="60">
         <v>44218</v>
       </c>
-      <c r="AL5" s="46"/>
-      <c r="AM5" s="45">
+      <c r="AL5" s="60"/>
+      <c r="AM5" s="59">
         <v>44225</v>
       </c>
-      <c r="AN5" s="45"/>
-      <c r="AO5" s="47">
+      <c r="AN5" s="59"/>
+      <c r="AO5" s="61">
         <v>44232</v>
       </c>
-      <c r="AP5" s="41"/>
-      <c r="AQ5" s="42">
+      <c r="AP5" s="62"/>
+      <c r="AQ5" s="63">
         <v>44239</v>
       </c>
-      <c r="AR5" s="42"/>
-      <c r="AS5" s="41">
+      <c r="AR5" s="63"/>
+      <c r="AS5" s="62">
         <v>44246</v>
       </c>
-      <c r="AT5" s="41"/>
-      <c r="AU5" s="42">
+      <c r="AT5" s="62"/>
+      <c r="AU5" s="63">
         <v>44253</v>
       </c>
-      <c r="AV5" s="42"/>
-      <c r="AW5" s="43">
+      <c r="AV5" s="63"/>
+      <c r="AW5" s="75">
         <v>44260</v>
       </c>
-      <c r="AX5" s="44"/>
-      <c r="AY5" s="37">
+      <c r="AX5" s="76"/>
+      <c r="AY5" s="71">
         <v>44267</v>
       </c>
-      <c r="AZ5" s="37"/>
-      <c r="BA5" s="44">
+      <c r="AZ5" s="71"/>
+      <c r="BA5" s="76">
         <v>44274</v>
       </c>
-      <c r="BB5" s="44"/>
-      <c r="BC5" s="37">
+      <c r="BB5" s="76"/>
+      <c r="BC5" s="71">
         <v>44281</v>
       </c>
-      <c r="BD5" s="38"/>
-      <c r="BE5" s="39">
+      <c r="BD5" s="72"/>
+      <c r="BE5" s="73">
         <v>44288</v>
       </c>
-      <c r="BF5" s="29"/>
-      <c r="BG5" s="40">
+      <c r="BF5" s="64"/>
+      <c r="BG5" s="74">
         <v>44295</v>
       </c>
-      <c r="BH5" s="40"/>
-      <c r="BI5" s="29">
+      <c r="BH5" s="74"/>
+      <c r="BI5" s="64">
         <v>44302</v>
       </c>
-      <c r="BJ5" s="29"/>
-      <c r="BK5" s="40">
+      <c r="BJ5" s="64"/>
+      <c r="BK5" s="74">
         <v>44309</v>
       </c>
-      <c r="BL5" s="40"/>
-      <c r="BM5" s="29">
+      <c r="BL5" s="74"/>
+      <c r="BM5" s="64">
         <v>44316</v>
       </c>
-      <c r="BN5" s="30"/>
-      <c r="BO5" s="73">
+      <c r="BN5" s="65"/>
+      <c r="BO5" s="29">
         <v>44323</v>
       </c>
-      <c r="BP5" s="74"/>
-      <c r="BQ5" s="75">
+      <c r="BP5" s="30"/>
+      <c r="BQ5" s="31">
         <v>44330</v>
       </c>
-      <c r="BR5" s="76"/>
+      <c r="BR5" s="32"/>
     </row>
     <row r="6" spans="2:70" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="61"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
       <c r="I6" s="19">
         <v>1</v>
       </c>
@@ -1820,10 +1820,10 @@
       </c>
     </row>
     <row r="7" spans="2:70" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="34"/>
+      <c r="C7" s="48"/>
       <c r="D7" s="4">
         <v>8</v>
       </c>
@@ -1843,10 +1843,10 @@
       <c r="J7" s="22"/>
     </row>
     <row r="8" spans="2:70" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="34"/>
+      <c r="C8" s="48"/>
       <c r="D8" s="4">
         <v>41</v>
       </c>
@@ -1866,10 +1866,10 @@
       <c r="J8" s="21"/>
     </row>
     <row r="9" spans="2:70" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="34"/>
+      <c r="C9" s="48"/>
       <c r="D9" s="4">
         <v>1</v>
       </c>
@@ -1889,10 +1889,10 @@
       <c r="J9" s="21"/>
     </row>
     <row r="10" spans="2:70" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="59" t="s">
+      <c r="B10" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="59"/>
+      <c r="C10" s="49"/>
       <c r="D10" s="27">
         <v>1</v>
       </c>
@@ -2004,10 +2004,10 @@
       <c r="J14" s="21"/>
     </row>
     <row r="15" spans="2:70" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="59" t="s">
+      <c r="B15" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="59"/>
+      <c r="C15" s="49"/>
       <c r="D15" s="27">
         <v>5</v>
       </c>
@@ -2188,10 +2188,10 @@
       <c r="J22" s="21"/>
     </row>
     <row r="23" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="59" t="s">
+      <c r="B23" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="59"/>
+      <c r="C23" s="49"/>
       <c r="D23" s="27">
         <v>19</v>
       </c>
@@ -2382,12 +2382,8 @@
       <c r="E31" s="4">
         <v>2</v>
       </c>
-      <c r="F31" s="4">
-        <v>56</v>
-      </c>
-      <c r="G31" s="4">
-        <v>2</v>
-      </c>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
       <c r="H31" s="5">
         <v>0</v>
       </c>
@@ -2418,10 +2414,10 @@
       <c r="J32" s="21"/>
     </row>
     <row r="33" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="59" t="s">
+      <c r="B33" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="59"/>
+      <c r="C33" s="49"/>
       <c r="D33" s="27">
         <v>33</v>
       </c>
@@ -2498,10 +2494,10 @@
       <c r="J36" s="21"/>
     </row>
     <row r="37" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="55" t="s">
+      <c r="B37" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="55"/>
+      <c r="C37" s="43"/>
       <c r="D37" s="27">
         <v>41</v>
       </c>
@@ -2575,13 +2571,27 @@
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="BO5:BP5"/>
-    <mergeCell ref="BQ5:BR5"/>
-    <mergeCell ref="AJ2:AQ2"/>
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="AB2:AH2"/>
+    <mergeCell ref="AQ5:AR5"/>
+    <mergeCell ref="BM5:BN5"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B4:C6"/>
+    <mergeCell ref="BC5:BD5"/>
+    <mergeCell ref="BE5:BF5"/>
+    <mergeCell ref="BG5:BH5"/>
+    <mergeCell ref="BI5:BJ5"/>
+    <mergeCell ref="BK5:BL5"/>
+    <mergeCell ref="AS5:AT5"/>
+    <mergeCell ref="AU5:AV5"/>
+    <mergeCell ref="AW5:AX5"/>
+    <mergeCell ref="AY5:AZ5"/>
+    <mergeCell ref="BA5:BB5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="AK5:AL5"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="AO5:AP5"/>
     <mergeCell ref="B37:C37"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="K5:L5"/>
@@ -2596,6 +2606,14 @@
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D4:D6"/>
     <mergeCell ref="E4:E6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="BO5:BP5"/>
+    <mergeCell ref="BQ5:BR5"/>
+    <mergeCell ref="AJ2:AQ2"/>
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="AB2:AH2"/>
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="Q5:R5"/>
     <mergeCell ref="S5:T5"/>
@@ -2605,28 +2623,6 @@
     <mergeCell ref="AA5:AB5"/>
     <mergeCell ref="AC5:AD5"/>
     <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="AK5:AL5"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="AO5:AP5"/>
-    <mergeCell ref="AQ5:AR5"/>
-    <mergeCell ref="BM5:BN5"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B4:C6"/>
-    <mergeCell ref="BC5:BD5"/>
-    <mergeCell ref="BE5:BF5"/>
-    <mergeCell ref="BG5:BH5"/>
-    <mergeCell ref="BI5:BJ5"/>
-    <mergeCell ref="BK5:BL5"/>
-    <mergeCell ref="AS5:AT5"/>
-    <mergeCell ref="AU5:AV5"/>
-    <mergeCell ref="AW5:AX5"/>
-    <mergeCell ref="AY5:AZ5"/>
-    <mergeCell ref="BA5:BB5"/>
   </mergeCells>
   <conditionalFormatting sqref="I7:BP40">
     <cfRule type="expression" dxfId="9" priority="1">

</xml_diff>

<commit_message>
Added a modal to Scg component that renders a from modal props stored in state. When this is undefined, there is no modal. Used this modal to let users choose between 2 skills when they gain a bonus that allows them to do that.
</commit_message>
<xml_diff>
--- a/documentation/Interim Report/Gantt Chart.xlsx
+++ b/documentation/Interim Report/Gantt Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domin\Documents\University\CO3201\documentation\Interim Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D00869-B78F-45C6-B756-9C4ED9D718C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC9A9CDB-6045-400A-B9D3-4DAD9426201A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25490" yWindow="-2940" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1680" yWindow="1035" windowWidth="10725" windowHeight="10290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -798,6 +798,90 @@
     <xf numFmtId="9" fontId="5" fillId="20" borderId="0" xfId="6" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="13" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="19" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="19" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="12" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="19" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="19" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="17" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="18" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="18" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="16" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="17" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="13" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="13" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="13" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="14" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="16" fontId="0" fillId="21" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -840,36 +924,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="13" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="13" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="13" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="14" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="16" fontId="13" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -887,60 +941,6 @@
     </xf>
     <xf numFmtId="16" fontId="13" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="16" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="17" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="17" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="19" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="19" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="12" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="19" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="19" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="18" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="18" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1354,7 +1354,7 @@
   <dimension ref="B1:BR40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="S31" sqref="S31"/>
+      <selection activeCell="S25" sqref="S25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1380,62 +1380,62 @@
       <c r="H1" s="7"/>
     </row>
     <row r="2" spans="2:70" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="66" t="s">
+      <c r="C2" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="67" t="s">
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="68"/>
+      <c r="H2" s="34"/>
       <c r="I2" s="23">
         <v>60</v>
       </c>
       <c r="K2" s="8"/>
-      <c r="L2" s="35" t="s">
+      <c r="L2" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="36"/>
-      <c r="P2" s="37"/>
+      <c r="M2" s="64"/>
+      <c r="N2" s="64"/>
+      <c r="O2" s="64"/>
+      <c r="P2" s="65"/>
       <c r="Q2" s="9"/>
-      <c r="R2" s="35" t="s">
+      <c r="R2" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="38"/>
-      <c r="T2" s="38"/>
-      <c r="U2" s="37"/>
+      <c r="S2" s="66"/>
+      <c r="T2" s="66"/>
+      <c r="U2" s="65"/>
       <c r="V2" s="10"/>
-      <c r="W2" s="33" t="s">
+      <c r="W2" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="X2" s="34"/>
-      <c r="Y2" s="34"/>
-      <c r="Z2" s="39"/>
+      <c r="X2" s="62"/>
+      <c r="Y2" s="62"/>
+      <c r="Z2" s="67"/>
       <c r="AA2" s="11"/>
-      <c r="AB2" s="40" t="s">
+      <c r="AB2" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="AC2" s="41"/>
-      <c r="AD2" s="41"/>
-      <c r="AE2" s="41"/>
-      <c r="AF2" s="41"/>
-      <c r="AG2" s="41"/>
-      <c r="AH2" s="42"/>
+      <c r="AC2" s="69"/>
+      <c r="AD2" s="69"/>
+      <c r="AE2" s="69"/>
+      <c r="AF2" s="69"/>
+      <c r="AG2" s="69"/>
+      <c r="AH2" s="70"/>
       <c r="AI2" s="12"/>
-      <c r="AJ2" s="33" t="s">
+      <c r="AJ2" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="AK2" s="34"/>
-      <c r="AL2" s="34"/>
-      <c r="AM2" s="34"/>
-      <c r="AN2" s="34"/>
-      <c r="AO2" s="34"/>
-      <c r="AP2" s="34"/>
-      <c r="AQ2" s="34"/>
+      <c r="AK2" s="62"/>
+      <c r="AL2" s="62"/>
+      <c r="AM2" s="62"/>
+      <c r="AN2" s="62"/>
+      <c r="AO2" s="62"/>
+      <c r="AP2" s="62"/>
+      <c r="AQ2" s="62"/>
     </row>
     <row r="3" spans="2:70" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C3"/>
@@ -1466,23 +1466,23 @@
       <c r="AB3"/>
     </row>
     <row r="4" spans="2:70" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="69" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="69"/>
-      <c r="D4" s="50" t="s">
+      <c r="B4" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="36"/>
+      <c r="D4" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="50" t="s">
+      <c r="E4" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="50" t="s">
+      <c r="F4" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="50" t="s">
+      <c r="G4" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="52" t="s">
+      <c r="H4" s="56" t="s">
         <v>10</v>
       </c>
       <c r="I4" s="14" t="s">
@@ -1498,146 +1498,146 @@
       <c r="O4" s="13"/>
     </row>
     <row r="5" spans="2:70" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="44">
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="56"/>
+      <c r="I5" s="49">
         <v>44120</v>
       </c>
-      <c r="J5" s="45"/>
-      <c r="K5" s="45">
+      <c r="J5" s="50"/>
+      <c r="K5" s="50">
         <v>44127</v>
       </c>
-      <c r="L5" s="46"/>
-      <c r="M5" s="47">
+      <c r="L5" s="51"/>
+      <c r="M5" s="52">
         <v>44134</v>
       </c>
-      <c r="N5" s="47"/>
-      <c r="O5" s="47">
+      <c r="N5" s="52"/>
+      <c r="O5" s="52">
         <v>44141</v>
       </c>
-      <c r="P5" s="47"/>
-      <c r="Q5" s="47">
+      <c r="P5" s="52"/>
+      <c r="Q5" s="52">
         <v>44148</v>
       </c>
-      <c r="R5" s="47"/>
-      <c r="S5" s="53">
+      <c r="R5" s="52"/>
+      <c r="S5" s="71">
         <v>44155</v>
       </c>
-      <c r="T5" s="53"/>
-      <c r="U5" s="47">
+      <c r="T5" s="71"/>
+      <c r="U5" s="52">
         <v>44162</v>
       </c>
-      <c r="V5" s="54"/>
-      <c r="W5" s="55">
+      <c r="V5" s="72"/>
+      <c r="W5" s="73">
         <v>44169</v>
       </c>
-      <c r="X5" s="55"/>
-      <c r="Y5" s="56">
+      <c r="X5" s="73"/>
+      <c r="Y5" s="74">
         <v>44176</v>
       </c>
-      <c r="Z5" s="56"/>
-      <c r="AA5" s="55">
+      <c r="Z5" s="74"/>
+      <c r="AA5" s="73">
         <v>44183</v>
       </c>
-      <c r="AB5" s="55"/>
-      <c r="AC5" s="56">
+      <c r="AB5" s="73"/>
+      <c r="AC5" s="74">
         <v>44190</v>
       </c>
-      <c r="AD5" s="57"/>
-      <c r="AE5" s="58">
+      <c r="AD5" s="75"/>
+      <c r="AE5" s="76">
         <v>44197</v>
       </c>
-      <c r="AF5" s="59"/>
-      <c r="AG5" s="60">
+      <c r="AF5" s="46"/>
+      <c r="AG5" s="45">
         <v>44204</v>
       </c>
-      <c r="AH5" s="60"/>
-      <c r="AI5" s="59">
+      <c r="AH5" s="45"/>
+      <c r="AI5" s="46">
         <v>44211</v>
       </c>
-      <c r="AJ5" s="59"/>
-      <c r="AK5" s="60">
+      <c r="AJ5" s="46"/>
+      <c r="AK5" s="45">
         <v>44218</v>
       </c>
-      <c r="AL5" s="60"/>
-      <c r="AM5" s="59">
+      <c r="AL5" s="45"/>
+      <c r="AM5" s="46">
         <v>44225</v>
       </c>
-      <c r="AN5" s="59"/>
-      <c r="AO5" s="61">
+      <c r="AN5" s="46"/>
+      <c r="AO5" s="47">
         <v>44232</v>
       </c>
-      <c r="AP5" s="62"/>
-      <c r="AQ5" s="63">
+      <c r="AP5" s="42"/>
+      <c r="AQ5" s="29">
         <v>44239</v>
       </c>
-      <c r="AR5" s="63"/>
-      <c r="AS5" s="62">
+      <c r="AR5" s="29"/>
+      <c r="AS5" s="42">
         <v>44246</v>
       </c>
-      <c r="AT5" s="62"/>
-      <c r="AU5" s="63">
+      <c r="AT5" s="42"/>
+      <c r="AU5" s="29">
         <v>44253</v>
       </c>
-      <c r="AV5" s="63"/>
-      <c r="AW5" s="75">
+      <c r="AV5" s="29"/>
+      <c r="AW5" s="43">
         <v>44260</v>
       </c>
-      <c r="AX5" s="76"/>
-      <c r="AY5" s="71">
+      <c r="AX5" s="44"/>
+      <c r="AY5" s="38">
         <v>44267</v>
       </c>
-      <c r="AZ5" s="71"/>
-      <c r="BA5" s="76">
+      <c r="AZ5" s="38"/>
+      <c r="BA5" s="44">
         <v>44274</v>
       </c>
-      <c r="BB5" s="76"/>
-      <c r="BC5" s="71">
+      <c r="BB5" s="44"/>
+      <c r="BC5" s="38">
         <v>44281</v>
       </c>
-      <c r="BD5" s="72"/>
-      <c r="BE5" s="73">
+      <c r="BD5" s="39"/>
+      <c r="BE5" s="40">
         <v>44288</v>
       </c>
-      <c r="BF5" s="64"/>
-      <c r="BG5" s="74">
+      <c r="BF5" s="30"/>
+      <c r="BG5" s="41">
         <v>44295</v>
       </c>
-      <c r="BH5" s="74"/>
-      <c r="BI5" s="64">
+      <c r="BH5" s="41"/>
+      <c r="BI5" s="30">
         <v>44302</v>
       </c>
-      <c r="BJ5" s="64"/>
-      <c r="BK5" s="74">
+      <c r="BJ5" s="30"/>
+      <c r="BK5" s="41">
         <v>44309</v>
       </c>
-      <c r="BL5" s="74"/>
-      <c r="BM5" s="64">
+      <c r="BL5" s="41"/>
+      <c r="BM5" s="30">
         <v>44316</v>
       </c>
-      <c r="BN5" s="65"/>
-      <c r="BO5" s="29">
+      <c r="BN5" s="31"/>
+      <c r="BO5" s="57">
         <v>44323</v>
       </c>
-      <c r="BP5" s="30"/>
-      <c r="BQ5" s="31">
+      <c r="BP5" s="58"/>
+      <c r="BQ5" s="59">
         <v>44330</v>
       </c>
-      <c r="BR5" s="32"/>
+      <c r="BR5" s="60"/>
     </row>
     <row r="6" spans="2:70" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="70"/>
-      <c r="C6" s="70"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="51"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="55"/>
       <c r="I6" s="19">
         <v>1</v>
       </c>
@@ -1820,10 +1820,10 @@
       </c>
     </row>
     <row r="7" spans="2:70" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="48"/>
+      <c r="C7" s="35"/>
       <c r="D7" s="4">
         <v>8</v>
       </c>
@@ -1843,10 +1843,10 @@
       <c r="J7" s="22"/>
     </row>
     <row r="8" spans="2:70" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="48"/>
+      <c r="C8" s="35"/>
       <c r="D8" s="4">
         <v>41</v>
       </c>
@@ -1866,10 +1866,10 @@
       <c r="J8" s="21"/>
     </row>
     <row r="9" spans="2:70" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="48"/>
+      <c r="C9" s="35"/>
       <c r="D9" s="4">
         <v>1</v>
       </c>
@@ -1889,10 +1889,10 @@
       <c r="J9" s="21"/>
     </row>
     <row r="10" spans="2:70" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="49"/>
+      <c r="C10" s="53"/>
       <c r="D10" s="27">
         <v>1</v>
       </c>
@@ -2004,10 +2004,10 @@
       <c r="J14" s="21"/>
     </row>
     <row r="15" spans="2:70" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="49" t="s">
+      <c r="B15" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="49"/>
+      <c r="C15" s="53"/>
       <c r="D15" s="27">
         <v>5</v>
       </c>
@@ -2188,10 +2188,10 @@
       <c r="J22" s="21"/>
     </row>
     <row r="23" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="49" t="s">
+      <c r="B23" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="49"/>
+      <c r="C23" s="53"/>
       <c r="D23" s="27">
         <v>19</v>
       </c>
@@ -2414,10 +2414,10 @@
       <c r="J32" s="21"/>
     </row>
     <row r="33" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="49" t="s">
+      <c r="B33" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="49"/>
+      <c r="C33" s="53"/>
       <c r="D33" s="27">
         <v>33</v>
       </c>
@@ -2482,7 +2482,7 @@
         <v>4</v>
       </c>
       <c r="F36" s="4">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G36" s="4">
         <v>2</v>
@@ -2494,10 +2494,10 @@
       <c r="J36" s="21"/>
     </row>
     <row r="37" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="43" t="s">
+      <c r="B37" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="43"/>
+      <c r="C37" s="48"/>
       <c r="D37" s="27">
         <v>41</v>
       </c>
@@ -2571,6 +2571,42 @@
     </row>
   </sheetData>
   <mergeCells count="52">
+    <mergeCell ref="BO5:BP5"/>
+    <mergeCell ref="BQ5:BR5"/>
+    <mergeCell ref="AJ2:AQ2"/>
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="AB2:AH2"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="AK5:AL5"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="AO5:AP5"/>
     <mergeCell ref="AQ5:AR5"/>
     <mergeCell ref="BM5:BN5"/>
     <mergeCell ref="C2:F2"/>
@@ -2587,42 +2623,6 @@
     <mergeCell ref="AW5:AX5"/>
     <mergeCell ref="AY5:AZ5"/>
     <mergeCell ref="BA5:BB5"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="AK5:AL5"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="AO5:AP5"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="H4:H6"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="BO5:BP5"/>
-    <mergeCell ref="BQ5:BR5"/>
-    <mergeCell ref="AJ2:AQ2"/>
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="AB2:AH2"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AE5:AF5"/>
   </mergeCells>
   <conditionalFormatting sqref="I7:BP40">
     <cfRule type="expression" dxfId="9" priority="1">

</xml_diff>

<commit_message>
Now able to export to pdf. Created form fillable pdf character sheet template. Wrote functions to extract data from character for each field in the sheet. Client requests the template, fills it out, then allows it to be saved
</commit_message>
<xml_diff>
--- a/documentation/Interim Report/Gantt Chart.xlsx
+++ b/documentation/Interim Report/Gantt Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domin\Documents\University\CO3201\documentation\Interim Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC9A9CDB-6045-400A-B9D3-4DAD9426201A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17873A1-51B8-4FAD-BB49-24DB2BA80498}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1680" yWindow="1035" windowWidth="10725" windowHeight="10290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -228,9 +228,6 @@
     <t>Build  SCG UI</t>
   </si>
   <si>
-    <t>Make physical sheet imitation UI (minimap)</t>
-  </si>
-  <si>
     <t>Users can create accounts and login</t>
   </si>
   <si>
@@ -247,6 +244,9 @@
   </si>
   <si>
     <t>Equipment panel</t>
+  </si>
+  <si>
+    <t>UI Overhaul</t>
   </si>
 </sst>
 </file>
@@ -798,6 +798,108 @@
     <xf numFmtId="9" fontId="5" fillId="20" borderId="0" xfId="6" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="21" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="21" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="21" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="14" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="14" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="15" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="15" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="13" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="13" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="13" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="16" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="17" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="17" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="16" fontId="13" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -816,9 +918,6 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -837,110 +936,11 @@
     <xf numFmtId="16" fontId="13" fillId="19" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="9" fillId="17" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="16" fontId="9" fillId="18" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="16" fontId="9" fillId="18" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="16" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="17" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="13" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="13" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="13" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="14" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="21" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="21" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="21" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="14" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="15" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="15" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1354,7 +1354,7 @@
   <dimension ref="B1:BR40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="S25" sqref="S25"/>
+      <selection activeCell="BS17" sqref="BS17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1380,62 +1380,62 @@
       <c r="H1" s="7"/>
     </row>
     <row r="2" spans="2:70" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="33" t="s">
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="34"/>
+      <c r="H2" s="68"/>
       <c r="I2" s="23">
         <v>60</v>
       </c>
       <c r="K2" s="8"/>
-      <c r="L2" s="63" t="s">
+      <c r="L2" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
-      <c r="O2" s="64"/>
-      <c r="P2" s="65"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="37"/>
       <c r="Q2" s="9"/>
-      <c r="R2" s="63" t="s">
+      <c r="R2" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="66"/>
-      <c r="T2" s="66"/>
-      <c r="U2" s="65"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="37"/>
       <c r="V2" s="10"/>
-      <c r="W2" s="61" t="s">
+      <c r="W2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="X2" s="62"/>
-      <c r="Y2" s="62"/>
-      <c r="Z2" s="67"/>
+      <c r="X2" s="34"/>
+      <c r="Y2" s="34"/>
+      <c r="Z2" s="39"/>
       <c r="AA2" s="11"/>
-      <c r="AB2" s="68" t="s">
+      <c r="AB2" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="AC2" s="69"/>
-      <c r="AD2" s="69"/>
-      <c r="AE2" s="69"/>
-      <c r="AF2" s="69"/>
-      <c r="AG2" s="69"/>
-      <c r="AH2" s="70"/>
+      <c r="AC2" s="41"/>
+      <c r="AD2" s="41"/>
+      <c r="AE2" s="41"/>
+      <c r="AF2" s="41"/>
+      <c r="AG2" s="41"/>
+      <c r="AH2" s="42"/>
       <c r="AI2" s="12"/>
-      <c r="AJ2" s="61" t="s">
+      <c r="AJ2" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="AK2" s="62"/>
-      <c r="AL2" s="62"/>
-      <c r="AM2" s="62"/>
-      <c r="AN2" s="62"/>
-      <c r="AO2" s="62"/>
-      <c r="AP2" s="62"/>
-      <c r="AQ2" s="62"/>
+      <c r="AK2" s="34"/>
+      <c r="AL2" s="34"/>
+      <c r="AM2" s="34"/>
+      <c r="AN2" s="34"/>
+      <c r="AO2" s="34"/>
+      <c r="AP2" s="34"/>
+      <c r="AQ2" s="34"/>
     </row>
     <row r="3" spans="2:70" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C3"/>
@@ -1466,23 +1466,23 @@
       <c r="AB3"/>
     </row>
     <row r="4" spans="2:70" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="54" t="s">
+      <c r="B4" s="69" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="69"/>
+      <c r="D4" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="54" t="s">
+      <c r="E4" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="54" t="s">
+      <c r="F4" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="54" t="s">
+      <c r="G4" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="56" t="s">
+      <c r="H4" s="59" t="s">
         <v>10</v>
       </c>
       <c r="I4" s="14" t="s">
@@ -1498,146 +1498,146 @@
       <c r="O4" s="13"/>
     </row>
     <row r="5" spans="2:70" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="56"/>
-      <c r="I5" s="49">
+      <c r="B5" s="69"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="52">
         <v>44120</v>
       </c>
-      <c r="J5" s="50"/>
-      <c r="K5" s="50">
+      <c r="J5" s="53"/>
+      <c r="K5" s="53">
         <v>44127</v>
       </c>
-      <c r="L5" s="51"/>
-      <c r="M5" s="52">
+      <c r="L5" s="54"/>
+      <c r="M5" s="43">
         <v>44134</v>
       </c>
-      <c r="N5" s="52"/>
-      <c r="O5" s="52">
+      <c r="N5" s="43"/>
+      <c r="O5" s="43">
         <v>44141</v>
       </c>
-      <c r="P5" s="52"/>
-      <c r="Q5" s="52">
+      <c r="P5" s="43"/>
+      <c r="Q5" s="43">
         <v>44148</v>
       </c>
-      <c r="R5" s="52"/>
-      <c r="S5" s="71">
+      <c r="R5" s="43"/>
+      <c r="S5" s="44">
         <v>44155</v>
       </c>
-      <c r="T5" s="71"/>
-      <c r="U5" s="52">
+      <c r="T5" s="44"/>
+      <c r="U5" s="43">
         <v>44162</v>
       </c>
-      <c r="V5" s="72"/>
-      <c r="W5" s="73">
+      <c r="V5" s="45"/>
+      <c r="W5" s="46">
         <v>44169</v>
       </c>
-      <c r="X5" s="73"/>
-      <c r="Y5" s="74">
+      <c r="X5" s="46"/>
+      <c r="Y5" s="47">
         <v>44176</v>
       </c>
-      <c r="Z5" s="74"/>
-      <c r="AA5" s="73">
+      <c r="Z5" s="47"/>
+      <c r="AA5" s="46">
         <v>44183</v>
       </c>
-      <c r="AB5" s="73"/>
-      <c r="AC5" s="74">
+      <c r="AB5" s="46"/>
+      <c r="AC5" s="47">
         <v>44190</v>
       </c>
-      <c r="AD5" s="75"/>
-      <c r="AE5" s="76">
+      <c r="AD5" s="48"/>
+      <c r="AE5" s="49">
         <v>44197</v>
       </c>
-      <c r="AF5" s="46"/>
-      <c r="AG5" s="45">
+      <c r="AF5" s="50"/>
+      <c r="AG5" s="60">
         <v>44204</v>
       </c>
-      <c r="AH5" s="45"/>
-      <c r="AI5" s="46">
+      <c r="AH5" s="60"/>
+      <c r="AI5" s="50">
         <v>44211</v>
       </c>
-      <c r="AJ5" s="46"/>
-      <c r="AK5" s="45">
+      <c r="AJ5" s="50"/>
+      <c r="AK5" s="60">
         <v>44218</v>
       </c>
-      <c r="AL5" s="45"/>
-      <c r="AM5" s="46">
+      <c r="AL5" s="60"/>
+      <c r="AM5" s="50">
         <v>44225</v>
       </c>
-      <c r="AN5" s="46"/>
-      <c r="AO5" s="47">
+      <c r="AN5" s="50"/>
+      <c r="AO5" s="61">
         <v>44232</v>
       </c>
-      <c r="AP5" s="42"/>
-      <c r="AQ5" s="29">
+      <c r="AP5" s="62"/>
+      <c r="AQ5" s="63">
         <v>44239</v>
       </c>
-      <c r="AR5" s="29"/>
-      <c r="AS5" s="42">
+      <c r="AR5" s="63"/>
+      <c r="AS5" s="62">
         <v>44246</v>
       </c>
-      <c r="AT5" s="42"/>
-      <c r="AU5" s="29">
+      <c r="AT5" s="62"/>
+      <c r="AU5" s="63">
         <v>44253</v>
       </c>
-      <c r="AV5" s="29"/>
-      <c r="AW5" s="43">
+      <c r="AV5" s="63"/>
+      <c r="AW5" s="75">
         <v>44260</v>
       </c>
-      <c r="AX5" s="44"/>
-      <c r="AY5" s="38">
+      <c r="AX5" s="76"/>
+      <c r="AY5" s="71">
         <v>44267</v>
       </c>
-      <c r="AZ5" s="38"/>
-      <c r="BA5" s="44">
+      <c r="AZ5" s="71"/>
+      <c r="BA5" s="76">
         <v>44274</v>
       </c>
-      <c r="BB5" s="44"/>
-      <c r="BC5" s="38">
+      <c r="BB5" s="76"/>
+      <c r="BC5" s="71">
         <v>44281</v>
       </c>
-      <c r="BD5" s="39"/>
-      <c r="BE5" s="40">
+      <c r="BD5" s="72"/>
+      <c r="BE5" s="73">
         <v>44288</v>
       </c>
-      <c r="BF5" s="30"/>
-      <c r="BG5" s="41">
+      <c r="BF5" s="64"/>
+      <c r="BG5" s="74">
         <v>44295</v>
       </c>
-      <c r="BH5" s="41"/>
-      <c r="BI5" s="30">
+      <c r="BH5" s="74"/>
+      <c r="BI5" s="64">
         <v>44302</v>
       </c>
-      <c r="BJ5" s="30"/>
-      <c r="BK5" s="41">
+      <c r="BJ5" s="64"/>
+      <c r="BK5" s="74">
         <v>44309</v>
       </c>
-      <c r="BL5" s="41"/>
-      <c r="BM5" s="30">
+      <c r="BL5" s="74"/>
+      <c r="BM5" s="64">
         <v>44316</v>
       </c>
-      <c r="BN5" s="31"/>
-      <c r="BO5" s="57">
+      <c r="BN5" s="65"/>
+      <c r="BO5" s="29">
         <v>44323</v>
       </c>
-      <c r="BP5" s="58"/>
-      <c r="BQ5" s="59">
+      <c r="BP5" s="30"/>
+      <c r="BQ5" s="31">
         <v>44330</v>
       </c>
-      <c r="BR5" s="60"/>
+      <c r="BR5" s="32"/>
     </row>
     <row r="6" spans="2:70" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="58"/>
       <c r="I6" s="19">
         <v>1</v>
       </c>
@@ -1820,10 +1820,10 @@
       </c>
     </row>
     <row r="7" spans="2:70" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="35"/>
+      <c r="C7" s="55"/>
       <c r="D7" s="4">
         <v>8</v>
       </c>
@@ -1843,10 +1843,10 @@
       <c r="J7" s="22"/>
     </row>
     <row r="8" spans="2:70" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="35"/>
+      <c r="C8" s="55"/>
       <c r="D8" s="4">
         <v>41</v>
       </c>
@@ -1866,10 +1866,10 @@
       <c r="J8" s="21"/>
     </row>
     <row r="9" spans="2:70" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="35"/>
+      <c r="C9" s="55"/>
       <c r="D9" s="4">
         <v>1</v>
       </c>
@@ -1883,16 +1883,16 @@
         <v>59</v>
       </c>
       <c r="H9" s="5">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="I9" s="21"/>
       <c r="J9" s="21"/>
     </row>
     <row r="10" spans="2:70" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="53" t="s">
+      <c r="B10" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="53"/>
+      <c r="C10" s="56"/>
       <c r="D10" s="27">
         <v>1</v>
       </c>
@@ -2004,10 +2004,10 @@
       <c r="J14" s="21"/>
     </row>
     <row r="15" spans="2:70" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="53" t="s">
+      <c r="B15" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="53"/>
+      <c r="C15" s="56"/>
       <c r="D15" s="27">
         <v>5</v>
       </c>
@@ -2167,7 +2167,7 @@
     <row r="22" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="16"/>
       <c r="C22" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D22" s="4">
         <v>17</v>
@@ -2188,10 +2188,10 @@
       <c r="J22" s="21"/>
     </row>
     <row r="23" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="53" t="s">
+      <c r="B23" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="53"/>
+      <c r="C23" s="56"/>
       <c r="D23" s="27">
         <v>19</v>
       </c>
@@ -2351,7 +2351,7 @@
     <row r="30" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="18"/>
       <c r="C30" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D30" s="4">
         <v>27</v>
@@ -2374,7 +2374,7 @@
     <row r="31" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="18"/>
       <c r="C31" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D31" s="4">
         <v>28</v>
@@ -2408,16 +2408,16 @@
         <v>2</v>
       </c>
       <c r="H32" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I32" s="21"/>
       <c r="J32" s="21"/>
     </row>
     <row r="33" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="53" t="s">
+      <c r="B33" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="53"/>
+      <c r="C33" s="56"/>
       <c r="D33" s="27">
         <v>33</v>
       </c>
@@ -2473,7 +2473,7 @@
     <row r="36" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="18"/>
       <c r="C36" s="15" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="D36" s="4">
         <v>37</v>
@@ -2494,10 +2494,10 @@
       <c r="J36" s="21"/>
     </row>
     <row r="37" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="C37" s="48"/>
+      <c r="B37" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" s="51"/>
       <c r="D37" s="27">
         <v>41</v>
       </c>
@@ -2515,7 +2515,7 @@
     <row r="38" spans="2:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="24"/>
       <c r="C38" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D38" s="4">
         <v>41</v>
@@ -2534,7 +2534,7 @@
     <row r="39" spans="2:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="24"/>
       <c r="C39" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D39" s="4">
         <v>43</v>
@@ -2553,7 +2553,7 @@
     <row r="40" spans="2:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="26"/>
       <c r="C40" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D40" s="4">
         <v>47</v>
@@ -2571,6 +2571,42 @@
     </row>
   </sheetData>
   <mergeCells count="52">
+    <mergeCell ref="AQ5:AR5"/>
+    <mergeCell ref="BM5:BN5"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B4:C6"/>
+    <mergeCell ref="BC5:BD5"/>
+    <mergeCell ref="BE5:BF5"/>
+    <mergeCell ref="BG5:BH5"/>
+    <mergeCell ref="BI5:BJ5"/>
+    <mergeCell ref="BK5:BL5"/>
+    <mergeCell ref="AS5:AT5"/>
+    <mergeCell ref="AU5:AV5"/>
+    <mergeCell ref="AW5:AX5"/>
+    <mergeCell ref="AY5:AZ5"/>
+    <mergeCell ref="BA5:BB5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="AK5:AL5"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="AO5:AP5"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="B8:C8"/>
     <mergeCell ref="BO5:BP5"/>
     <mergeCell ref="BQ5:BR5"/>
     <mergeCell ref="AJ2:AQ2"/>
@@ -2587,42 +2623,6 @@
     <mergeCell ref="AA5:AB5"/>
     <mergeCell ref="AC5:AD5"/>
     <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="H4:H6"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="AK5:AL5"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="AO5:AP5"/>
-    <mergeCell ref="AQ5:AR5"/>
-    <mergeCell ref="BM5:BN5"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B4:C6"/>
-    <mergeCell ref="BC5:BD5"/>
-    <mergeCell ref="BE5:BF5"/>
-    <mergeCell ref="BG5:BH5"/>
-    <mergeCell ref="BI5:BJ5"/>
-    <mergeCell ref="BK5:BL5"/>
-    <mergeCell ref="AS5:AT5"/>
-    <mergeCell ref="AU5:AV5"/>
-    <mergeCell ref="AW5:AX5"/>
-    <mergeCell ref="AY5:AZ5"/>
-    <mergeCell ref="BA5:BB5"/>
   </mergeCells>
   <conditionalFormatting sqref="I7:BP40">
     <cfRule type="expression" dxfId="9" priority="1">

</xml_diff>

<commit_message>
Reformatted ClassAvatar to be a neater rsuite panel. Changed class panel to be a PanelGroup of class avatars
</commit_message>
<xml_diff>
--- a/documentation/Interim Report/Gantt Chart.xlsx
+++ b/documentation/Interim Report/Gantt Chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domin\Documents\University\CO3201\documentation\Interim Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17873A1-51B8-4FAD-BB49-24DB2BA80498}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F3F9FA-7AE1-49DE-8A7F-753C1E7B5CB4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25490" yWindow="-2940" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -798,6 +798,90 @@
     <xf numFmtId="9" fontId="5" fillId="20" borderId="0" xfId="6" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="13" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="19" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="19" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="12" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="19" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="19" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="17" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="18" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="18" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="16" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="17" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="13" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="13" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="13" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="14" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="16" fontId="0" fillId="21" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -840,9 +924,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="9" fillId="14" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="16" fontId="13" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -860,87 +941,6 @@
     </xf>
     <xf numFmtId="16" fontId="13" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="13" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="13" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="13" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="16" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="17" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="17" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="19" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="19" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="12" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="19" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="13" fillId="19" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="18" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="18" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1354,7 +1354,7 @@
   <dimension ref="B1:BR40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="BS17" sqref="BS17"/>
+      <selection activeCell="V36" sqref="V36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1380,62 +1380,62 @@
       <c r="H1" s="7"/>
     </row>
     <row r="2" spans="2:70" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="66" t="s">
+      <c r="C2" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="67" t="s">
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="68"/>
+      <c r="H2" s="34"/>
       <c r="I2" s="23">
         <v>60</v>
       </c>
       <c r="K2" s="8"/>
-      <c r="L2" s="35" t="s">
+      <c r="L2" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="36"/>
-      <c r="P2" s="37"/>
+      <c r="M2" s="64"/>
+      <c r="N2" s="64"/>
+      <c r="O2" s="64"/>
+      <c r="P2" s="65"/>
       <c r="Q2" s="9"/>
-      <c r="R2" s="35" t="s">
+      <c r="R2" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="38"/>
-      <c r="T2" s="38"/>
-      <c r="U2" s="37"/>
+      <c r="S2" s="66"/>
+      <c r="T2" s="66"/>
+      <c r="U2" s="65"/>
       <c r="V2" s="10"/>
-      <c r="W2" s="33" t="s">
+      <c r="W2" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="X2" s="34"/>
-      <c r="Y2" s="34"/>
-      <c r="Z2" s="39"/>
+      <c r="X2" s="62"/>
+      <c r="Y2" s="62"/>
+      <c r="Z2" s="67"/>
       <c r="AA2" s="11"/>
-      <c r="AB2" s="40" t="s">
+      <c r="AB2" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="AC2" s="41"/>
-      <c r="AD2" s="41"/>
-      <c r="AE2" s="41"/>
-      <c r="AF2" s="41"/>
-      <c r="AG2" s="41"/>
-      <c r="AH2" s="42"/>
+      <c r="AC2" s="69"/>
+      <c r="AD2" s="69"/>
+      <c r="AE2" s="69"/>
+      <c r="AF2" s="69"/>
+      <c r="AG2" s="69"/>
+      <c r="AH2" s="70"/>
       <c r="AI2" s="12"/>
-      <c r="AJ2" s="33" t="s">
+      <c r="AJ2" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="AK2" s="34"/>
-      <c r="AL2" s="34"/>
-      <c r="AM2" s="34"/>
-      <c r="AN2" s="34"/>
-      <c r="AO2" s="34"/>
-      <c r="AP2" s="34"/>
-      <c r="AQ2" s="34"/>
+      <c r="AK2" s="62"/>
+      <c r="AL2" s="62"/>
+      <c r="AM2" s="62"/>
+      <c r="AN2" s="62"/>
+      <c r="AO2" s="62"/>
+      <c r="AP2" s="62"/>
+      <c r="AQ2" s="62"/>
     </row>
     <row r="3" spans="2:70" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C3"/>
@@ -1466,23 +1466,23 @@
       <c r="AB3"/>
     </row>
     <row r="4" spans="2:70" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="69" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="69"/>
-      <c r="D4" s="57" t="s">
+      <c r="B4" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="36"/>
+      <c r="D4" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="57" t="s">
+      <c r="E4" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="57" t="s">
+      <c r="F4" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="57" t="s">
+      <c r="G4" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="59" t="s">
+      <c r="H4" s="56" t="s">
         <v>10</v>
       </c>
       <c r="I4" s="14" t="s">
@@ -1498,146 +1498,146 @@
       <c r="O4" s="13"/>
     </row>
     <row r="5" spans="2:70" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="57"/>
-      <c r="H5" s="59"/>
-      <c r="I5" s="52">
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="56"/>
+      <c r="I5" s="49">
         <v>44120</v>
       </c>
-      <c r="J5" s="53"/>
-      <c r="K5" s="53">
+      <c r="J5" s="50"/>
+      <c r="K5" s="50">
         <v>44127</v>
       </c>
-      <c r="L5" s="54"/>
-      <c r="M5" s="43">
+      <c r="L5" s="51"/>
+      <c r="M5" s="52">
         <v>44134</v>
       </c>
-      <c r="N5" s="43"/>
-      <c r="O5" s="43">
+      <c r="N5" s="52"/>
+      <c r="O5" s="52">
         <v>44141</v>
       </c>
-      <c r="P5" s="43"/>
-      <c r="Q5" s="43">
+      <c r="P5" s="52"/>
+      <c r="Q5" s="52">
         <v>44148</v>
       </c>
-      <c r="R5" s="43"/>
-      <c r="S5" s="44">
+      <c r="R5" s="52"/>
+      <c r="S5" s="71">
         <v>44155</v>
       </c>
-      <c r="T5" s="44"/>
-      <c r="U5" s="43">
+      <c r="T5" s="71"/>
+      <c r="U5" s="52">
         <v>44162</v>
       </c>
-      <c r="V5" s="45"/>
-      <c r="W5" s="46">
+      <c r="V5" s="72"/>
+      <c r="W5" s="73">
         <v>44169</v>
       </c>
-      <c r="X5" s="46"/>
-      <c r="Y5" s="47">
+      <c r="X5" s="73"/>
+      <c r="Y5" s="74">
         <v>44176</v>
       </c>
-      <c r="Z5" s="47"/>
-      <c r="AA5" s="46">
+      <c r="Z5" s="74"/>
+      <c r="AA5" s="73">
         <v>44183</v>
       </c>
-      <c r="AB5" s="46"/>
-      <c r="AC5" s="47">
+      <c r="AB5" s="73"/>
+      <c r="AC5" s="74">
         <v>44190</v>
       </c>
-      <c r="AD5" s="48"/>
-      <c r="AE5" s="49">
+      <c r="AD5" s="75"/>
+      <c r="AE5" s="76">
         <v>44197</v>
       </c>
-      <c r="AF5" s="50"/>
-      <c r="AG5" s="60">
+      <c r="AF5" s="46"/>
+      <c r="AG5" s="45">
         <v>44204</v>
       </c>
-      <c r="AH5" s="60"/>
-      <c r="AI5" s="50">
+      <c r="AH5" s="45"/>
+      <c r="AI5" s="46">
         <v>44211</v>
       </c>
-      <c r="AJ5" s="50"/>
-      <c r="AK5" s="60">
+      <c r="AJ5" s="46"/>
+      <c r="AK5" s="45">
         <v>44218</v>
       </c>
-      <c r="AL5" s="60"/>
-      <c r="AM5" s="50">
+      <c r="AL5" s="45"/>
+      <c r="AM5" s="46">
         <v>44225</v>
       </c>
-      <c r="AN5" s="50"/>
-      <c r="AO5" s="61">
+      <c r="AN5" s="46"/>
+      <c r="AO5" s="47">
         <v>44232</v>
       </c>
-      <c r="AP5" s="62"/>
-      <c r="AQ5" s="63">
+      <c r="AP5" s="42"/>
+      <c r="AQ5" s="29">
         <v>44239</v>
       </c>
-      <c r="AR5" s="63"/>
-      <c r="AS5" s="62">
+      <c r="AR5" s="29"/>
+      <c r="AS5" s="42">
         <v>44246</v>
       </c>
-      <c r="AT5" s="62"/>
-      <c r="AU5" s="63">
+      <c r="AT5" s="42"/>
+      <c r="AU5" s="29">
         <v>44253</v>
       </c>
-      <c r="AV5" s="63"/>
-      <c r="AW5" s="75">
+      <c r="AV5" s="29"/>
+      <c r="AW5" s="43">
         <v>44260</v>
       </c>
-      <c r="AX5" s="76"/>
-      <c r="AY5" s="71">
+      <c r="AX5" s="44"/>
+      <c r="AY5" s="38">
         <v>44267</v>
       </c>
-      <c r="AZ5" s="71"/>
-      <c r="BA5" s="76">
+      <c r="AZ5" s="38"/>
+      <c r="BA5" s="44">
         <v>44274</v>
       </c>
-      <c r="BB5" s="76"/>
-      <c r="BC5" s="71">
+      <c r="BB5" s="44"/>
+      <c r="BC5" s="38">
         <v>44281</v>
       </c>
-      <c r="BD5" s="72"/>
-      <c r="BE5" s="73">
+      <c r="BD5" s="39"/>
+      <c r="BE5" s="40">
         <v>44288</v>
       </c>
-      <c r="BF5" s="64"/>
-      <c r="BG5" s="74">
+      <c r="BF5" s="30"/>
+      <c r="BG5" s="41">
         <v>44295</v>
       </c>
-      <c r="BH5" s="74"/>
-      <c r="BI5" s="64">
+      <c r="BH5" s="41"/>
+      <c r="BI5" s="30">
         <v>44302</v>
       </c>
-      <c r="BJ5" s="64"/>
-      <c r="BK5" s="74">
+      <c r="BJ5" s="30"/>
+      <c r="BK5" s="41">
         <v>44309</v>
       </c>
-      <c r="BL5" s="74"/>
-      <c r="BM5" s="64">
+      <c r="BL5" s="41"/>
+      <c r="BM5" s="30">
         <v>44316</v>
       </c>
-      <c r="BN5" s="65"/>
-      <c r="BO5" s="29">
+      <c r="BN5" s="31"/>
+      <c r="BO5" s="57">
         <v>44323</v>
       </c>
-      <c r="BP5" s="30"/>
-      <c r="BQ5" s="31">
+      <c r="BP5" s="58"/>
+      <c r="BQ5" s="59">
         <v>44330</v>
       </c>
-      <c r="BR5" s="32"/>
+      <c r="BR5" s="60"/>
     </row>
     <row r="6" spans="2:70" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="70"/>
-      <c r="C6" s="70"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="58"/>
-      <c r="G6" s="58"/>
-      <c r="H6" s="58"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="55"/>
       <c r="I6" s="19">
         <v>1</v>
       </c>
@@ -1820,10 +1820,10 @@
       </c>
     </row>
     <row r="7" spans="2:70" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="55" t="s">
+      <c r="B7" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="55"/>
+      <c r="C7" s="35"/>
       <c r="D7" s="4">
         <v>8</v>
       </c>
@@ -1843,10 +1843,10 @@
       <c r="J7" s="22"/>
     </row>
     <row r="8" spans="2:70" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="55" t="s">
+      <c r="B8" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="55"/>
+      <c r="C8" s="35"/>
       <c r="D8" s="4">
         <v>41</v>
       </c>
@@ -1866,10 +1866,10 @@
       <c r="J8" s="21"/>
     </row>
     <row r="9" spans="2:70" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="55" t="s">
+      <c r="B9" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="55"/>
+      <c r="C9" s="35"/>
       <c r="D9" s="4">
         <v>1</v>
       </c>
@@ -1889,10 +1889,10 @@
       <c r="J9" s="21"/>
     </row>
     <row r="10" spans="2:70" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="56"/>
+      <c r="C10" s="53"/>
       <c r="D10" s="27">
         <v>1</v>
       </c>
@@ -2004,10 +2004,10 @@
       <c r="J14" s="21"/>
     </row>
     <row r="15" spans="2:70" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="56" t="s">
+      <c r="B15" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="56"/>
+      <c r="C15" s="53"/>
       <c r="D15" s="27">
         <v>5</v>
       </c>
@@ -2188,10 +2188,10 @@
       <c r="J22" s="21"/>
     </row>
     <row r="23" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="56" t="s">
+      <c r="B23" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="56"/>
+      <c r="C23" s="53"/>
       <c r="D23" s="27">
         <v>19</v>
       </c>
@@ -2414,10 +2414,10 @@
       <c r="J32" s="21"/>
     </row>
     <row r="33" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="56" t="s">
+      <c r="B33" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="56"/>
+      <c r="C33" s="53"/>
       <c r="D33" s="27">
         <v>33</v>
       </c>
@@ -2485,19 +2485,19 @@
         <v>56</v>
       </c>
       <c r="G36" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H36" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I36" s="21"/>
       <c r="J36" s="21"/>
     </row>
     <row r="37" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="51" t="s">
+      <c r="B37" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="C37" s="51"/>
+      <c r="C37" s="48"/>
       <c r="D37" s="27">
         <v>41</v>
       </c>
@@ -2571,6 +2571,42 @@
     </row>
   </sheetData>
   <mergeCells count="52">
+    <mergeCell ref="BO5:BP5"/>
+    <mergeCell ref="BQ5:BR5"/>
+    <mergeCell ref="AJ2:AQ2"/>
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="AB2:AH2"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="AK5:AL5"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="AO5:AP5"/>
     <mergeCell ref="AQ5:AR5"/>
     <mergeCell ref="BM5:BN5"/>
     <mergeCell ref="C2:F2"/>
@@ -2587,42 +2623,6 @@
     <mergeCell ref="AW5:AX5"/>
     <mergeCell ref="AY5:AZ5"/>
     <mergeCell ref="BA5:BB5"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="AK5:AL5"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="AO5:AP5"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="H4:H6"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="BO5:BP5"/>
-    <mergeCell ref="BQ5:BR5"/>
-    <mergeCell ref="AJ2:AQ2"/>
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="AB2:AH2"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AE5:AF5"/>
   </mergeCells>
   <conditionalFormatting sqref="I7:BP40">
     <cfRule type="expression" dxfId="9" priority="1">

</xml_diff>